<commit_message>
c implementation and new local search
</commit_message>
<xml_diff>
--- a/results/comparison.xlsx
+++ b/results/comparison.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\radovi\K-domination\k-domination\algorithms\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\radovi\K-domination\k-domination\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="55">
   <si>
     <t>k=1</t>
   </si>
@@ -161,6 +161,30 @@
   </si>
   <si>
     <t>\hline</t>
+  </si>
+  <si>
+    <t>Lit (k=1)</t>
+  </si>
+  <si>
+    <t>VNS (k=1)</t>
+  </si>
+  <si>
+    <t>VNS (k=2)</t>
+  </si>
+  <si>
+    <t>Lit (k=2)</t>
+  </si>
+  <si>
+    <t>VNS (k=4)</t>
+  </si>
+  <si>
+    <t>Lit (k=4)</t>
+  </si>
+  <si>
+    <t>|V|</t>
+  </si>
+  <si>
+    <t>|E|</t>
   </si>
 </sst>
 </file>
@@ -251,6 +275,1175 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="sr-Latn-CS"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18308381959285941"/>
+          <c:y val="0.17964908310007832"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sr-Latn-RS"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'No. vertex and egg'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>|V|</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'No. vertex and egg'!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>Bath</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Belfast</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Brighton</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Bristol</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Cardiff</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Coventry</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Exeter</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Glasgow</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Leeds</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Leicester</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Liverpool</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Manchester</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Newcastle</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Nottingham</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Oxford</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Plymouth</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Sheffield</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Southampton</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Sunderland</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>York</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'No. vertex and egg'!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>910</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>976</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1569</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1127</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1175</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1137</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1647</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1531</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1273</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1109</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1739</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>479</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1122</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1582</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>796</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1346</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1044</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'No. vertex and egg'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>|E|</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'No. vertex and egg'!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>Bath</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Belfast</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Brighton</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Bristol</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Cardiff</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Coventry</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Exeter</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Glasgow</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Leeds</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Leicester</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Liverpool</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Manchester</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Newcastle</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Nottingham</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Oxford</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Plymouth</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Sheffield</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Southampton</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Sunderland</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>York</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'No. vertex and egg'!$C$2:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>18560</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62617</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47522</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23155</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26689</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24323</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>56511</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>48219</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42564</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>77286</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26614</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>51595</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8396</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>35070</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50534</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19942</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42013</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23774</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-905245152"/>
+        <c:axId val="-905239712"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-905245152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sr-Latn-RS"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-905239712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-905239712"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sr-Latn-RS"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-905245152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.83975439611458591"/>
+          <c:y val="0.16892627845254243"/>
+          <c:w val="0.12340661044528198"/>
+          <c:h val="9.0000629921259859E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sr-Latn-RS"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sr-Latn-RS"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>328611</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafikon 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -540,10 +1733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L86"/>
+  <dimension ref="A1:U86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:L28"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +1826,7 @@
         <v>0.9</v>
       </c>
       <c r="L4" t="str">
-        <f>A4&amp;"&amp;"&amp;'No. vertex and egg'!B1&amp;"&amp;"&amp;'No. vertex and egg'!C1&amp;"&amp;"&amp;IF(C4&lt;=I4,"\bf{"&amp;C4&amp;"}",C4)&amp;"&amp;"&amp;ROUND(D4,1)&amp;"&amp;"&amp;ROUND(E4,1)&amp;"&amp;"&amp;G4&amp;"&amp;"&amp;IF(I4&lt;=C4,"\bf{"&amp;I4&amp;"}",I4)&amp;"&amp;"&amp;ROUND(J4,1)&amp;"&amp;"&amp;IF(C33&lt;=I33,"\bf{"&amp;C33&amp;"}",C33)&amp;"&amp;"&amp;ROUND(D33,1)&amp;"&amp;"&amp;ROUND(E33,1)&amp;"&amp;"&amp;G33&amp;"&amp;"&amp;IF(I33&lt;=C33,"\bf{"&amp;I33&amp;"}",I33)&amp;"&amp;"&amp;ROUND(J33,1)&amp;"&amp;"&amp;IF(C62&lt;=I62,"\bf{"&amp;C62&amp;"}",C62)&amp;"&amp;"&amp;ROUND(D62,1)&amp;"&amp;"&amp;ROUND(E62,1)&amp;"&amp;"&amp;G62&amp;"&amp;"&amp;IF(I62&lt;=C62,"\bf{"&amp;I62&amp;"}",I62)&amp;"&amp;"&amp;ROUND(J62,1)&amp;"\\"</f>
+        <f>A4&amp;"&amp;"&amp;'No. vertex and egg'!B2&amp;"&amp;"&amp;'No. vertex and egg'!C2&amp;"&amp;"&amp;IF(C4&lt;=I4,"\bf{"&amp;C4&amp;"}",C4)&amp;"&amp;"&amp;ROUND(D4,1)&amp;"&amp;"&amp;ROUND(E4,1)&amp;"&amp;"&amp;G4&amp;"&amp;"&amp;IF(I4&lt;=C4,"\bf{"&amp;I4&amp;"}",I4)&amp;"&amp;"&amp;ROUND(J4,1)&amp;"&amp;"&amp;IF(C33&lt;=I33,"\bf{"&amp;C33&amp;"}",C33)&amp;"&amp;"&amp;ROUND(D33,1)&amp;"&amp;"&amp;ROUND(E33,1)&amp;"&amp;"&amp;G33&amp;"&amp;"&amp;IF(I33&lt;=C33,"\bf{"&amp;I33&amp;"}",I33)&amp;"&amp;"&amp;ROUND(J33,1)&amp;"&amp;"&amp;IF(C62&lt;=I62,"\bf{"&amp;C62&amp;"}",C62)&amp;"&amp;"&amp;ROUND(D62,1)&amp;"&amp;"&amp;ROUND(E62,1)&amp;"&amp;"&amp;G62&amp;"&amp;"&amp;IF(I62&lt;=C62,"\bf{"&amp;I62&amp;"}",I62)&amp;"&amp;"&amp;ROUND(J62,1)&amp;"\\"</f>
         <v>Bath&amp;910&amp;18560&amp;\bf{38}&amp;0&amp;661.7&amp;BS4&amp;44.6&amp;0.9&amp;\bf{71.1}&amp;0.3&amp;720.7&amp;BS1&amp;89&amp;1.4&amp;\bf{140.1}&amp;0.7&amp;644.8&amp;BS4&amp;160&amp;1.1\\</v>
       </c>
     </row>
@@ -669,7 +1862,7 @@
         <v>1.5</v>
       </c>
       <c r="L5" t="str">
-        <f>A5&amp;"&amp;"&amp;'No. vertex and egg'!B2&amp;"&amp;"&amp;'No. vertex and egg'!C2&amp;"&amp;"&amp;IF(C5&lt;=I5,"\bf{"&amp;C5&amp;"}",C5)&amp;"&amp;"&amp;ROUND(D5,1)&amp;"&amp;"&amp;ROUND(E5,1)&amp;"&amp;"&amp;G5&amp;"&amp;"&amp;IF(I5&lt;=C5,"\bf{"&amp;I5&amp;"}",I5)&amp;"&amp;"&amp;ROUND(J5,1)&amp;"&amp;"&amp;IF(C34&lt;=I34,"\bf{"&amp;C34&amp;"}",C34)&amp;"&amp;"&amp;ROUND(D34,1)&amp;"&amp;"&amp;ROUND(E34,1)&amp;"&amp;"&amp;G34&amp;"&amp;"&amp;IF(I34&lt;=C34,"\bf{"&amp;I34&amp;"}",I34)&amp;"&amp;"&amp;ROUND(J34,1)&amp;"&amp;"&amp;IF(C63&lt;=I63,"\bf{"&amp;C63&amp;"}",C63)&amp;"&amp;"&amp;ROUND(D63,1)&amp;"&amp;"&amp;ROUND(E63,1)&amp;"&amp;"&amp;G63&amp;"&amp;"&amp;IF(I63&lt;=C63,"\bf{"&amp;I63&amp;"}",I63)&amp;"&amp;"&amp;ROUND(J63,1)&amp;"\\"</f>
+        <f>A5&amp;"&amp;"&amp;'No. vertex and egg'!B3&amp;"&amp;"&amp;'No. vertex and egg'!C3&amp;"&amp;"&amp;IF(C5&lt;=I5,"\bf{"&amp;C5&amp;"}",C5)&amp;"&amp;"&amp;ROUND(D5,1)&amp;"&amp;"&amp;ROUND(E5,1)&amp;"&amp;"&amp;G5&amp;"&amp;"&amp;IF(I5&lt;=C5,"\bf{"&amp;I5&amp;"}",I5)&amp;"&amp;"&amp;ROUND(J5,1)&amp;"&amp;"&amp;IF(C34&lt;=I34,"\bf{"&amp;C34&amp;"}",C34)&amp;"&amp;"&amp;ROUND(D34,1)&amp;"&amp;"&amp;ROUND(E34,1)&amp;"&amp;"&amp;G34&amp;"&amp;"&amp;IF(I34&lt;=C34,"\bf{"&amp;I34&amp;"}",I34)&amp;"&amp;"&amp;ROUND(J34,1)&amp;"&amp;"&amp;IF(C63&lt;=I63,"\bf{"&amp;C63&amp;"}",C63)&amp;"&amp;"&amp;ROUND(D63,1)&amp;"&amp;"&amp;ROUND(E63,1)&amp;"&amp;"&amp;G63&amp;"&amp;"&amp;IF(I63&lt;=C63,"\bf{"&amp;I63&amp;"}",I63)&amp;"&amp;"&amp;ROUND(J63,1)&amp;"\\"</f>
         <v>Belfast&amp;1700&amp;62617&amp;\bf{39}&amp;0&amp;1800.1&amp;BS4&amp;50.2&amp;1.5&amp;\bf{76.3}&amp;0.5&amp;1800.3&amp;BS4&amp;97.6&amp;1&amp;\bf{148.3}&amp;0.7&amp;1800.1&amp;BS4&amp;179.6&amp;2\\</v>
       </c>
     </row>
@@ -705,7 +1898,7 @@
         <v>0.6</v>
       </c>
       <c r="L6" t="str">
-        <f>A6&amp;"&amp;"&amp;'No. vertex and egg'!B3&amp;"&amp;"&amp;'No. vertex and egg'!C3&amp;"&amp;"&amp;IF(C6&lt;=I6,"\bf{"&amp;C6&amp;"}",C6)&amp;"&amp;"&amp;ROUND(D6,1)&amp;"&amp;"&amp;ROUND(E6,1)&amp;"&amp;"&amp;G6&amp;"&amp;"&amp;IF(I6&lt;=C6,"\bf{"&amp;I6&amp;"}",I6)&amp;"&amp;"&amp;ROUND(J6,1)&amp;"&amp;"&amp;IF(C35&lt;=I35,"\bf{"&amp;C35&amp;"}",C35)&amp;"&amp;"&amp;ROUND(D35,1)&amp;"&amp;"&amp;ROUND(E35,1)&amp;"&amp;"&amp;G35&amp;"&amp;"&amp;IF(I35&lt;=C35,"\bf{"&amp;I35&amp;"}",I35)&amp;"&amp;"&amp;ROUND(J35,1)&amp;"&amp;"&amp;IF(C64&lt;=I64,"\bf{"&amp;C64&amp;"}",C64)&amp;"&amp;"&amp;ROUND(D64,1)&amp;"&amp;"&amp;ROUND(E64,1)&amp;"&amp;"&amp;G64&amp;"&amp;"&amp;IF(I64&lt;=C64,"\bf{"&amp;I64&amp;"}",I64)&amp;"&amp;"&amp;ROUND(J64,1)&amp;"\\"</f>
+        <f>A6&amp;"&amp;"&amp;'No. vertex and egg'!B4&amp;"&amp;"&amp;'No. vertex and egg'!C4&amp;"&amp;"&amp;IF(C6&lt;=I6,"\bf{"&amp;C6&amp;"}",C6)&amp;"&amp;"&amp;ROUND(D6,1)&amp;"&amp;"&amp;ROUND(E6,1)&amp;"&amp;"&amp;G6&amp;"&amp;"&amp;IF(I6&lt;=C6,"\bf{"&amp;I6&amp;"}",I6)&amp;"&amp;"&amp;ROUND(J6,1)&amp;"&amp;"&amp;IF(C35&lt;=I35,"\bf{"&amp;C35&amp;"}",C35)&amp;"&amp;"&amp;ROUND(D35,1)&amp;"&amp;"&amp;ROUND(E35,1)&amp;"&amp;"&amp;G35&amp;"&amp;"&amp;IF(I35&lt;=C35,"\bf{"&amp;I35&amp;"}",I35)&amp;"&amp;"&amp;ROUND(J35,1)&amp;"&amp;"&amp;IF(C64&lt;=I64,"\bf{"&amp;C64&amp;"}",C64)&amp;"&amp;"&amp;ROUND(D64,1)&amp;"&amp;"&amp;ROUND(E64,1)&amp;"&amp;"&amp;G64&amp;"&amp;"&amp;IF(I64&lt;=C64,"\bf{"&amp;I64&amp;"}",I64)&amp;"&amp;"&amp;ROUND(J64,1)&amp;"\\"</f>
         <v>Brighton&amp;976&amp;35012&amp;\bf{21}&amp;0&amp;1334&amp;BS4&amp;28.2&amp;0.6&amp;\bf{40.1}&amp;0.3&amp;1789.7&amp;BS4&amp;49.4&amp;0.5&amp;\bf{78}&amp;0.5&amp;1800.1&amp;BS4&amp;94.8&amp;1.9\\</v>
       </c>
     </row>
@@ -741,7 +1934,7 @@
         <v>1</v>
       </c>
       <c r="L7" t="str">
-        <f>A7&amp;"&amp;"&amp;'No. vertex and egg'!B4&amp;"&amp;"&amp;'No. vertex and egg'!C4&amp;"&amp;"&amp;IF(C7&lt;=I7,"\bf{"&amp;C7&amp;"}",C7)&amp;"&amp;"&amp;ROUND(D7,1)&amp;"&amp;"&amp;ROUND(E7,1)&amp;"&amp;"&amp;G7&amp;"&amp;"&amp;IF(I7&lt;=C7,"\bf{"&amp;I7&amp;"}",I7)&amp;"&amp;"&amp;ROUND(J7,1)&amp;"&amp;"&amp;IF(C36&lt;=I36,"\bf{"&amp;C36&amp;"}",C36)&amp;"&amp;"&amp;ROUND(D36,1)&amp;"&amp;"&amp;ROUND(E36,1)&amp;"&amp;"&amp;G36&amp;"&amp;"&amp;IF(I36&lt;=C36,"\bf{"&amp;I36&amp;"}",I36)&amp;"&amp;"&amp;ROUND(J36,1)&amp;"&amp;"&amp;IF(C65&lt;=I65,"\bf{"&amp;C65&amp;"}",C65)&amp;"&amp;"&amp;ROUND(D65,1)&amp;"&amp;"&amp;ROUND(E65,1)&amp;"&amp;"&amp;G65&amp;"&amp;"&amp;IF(I65&lt;=C65,"\bf{"&amp;I65&amp;"}",I65)&amp;"&amp;"&amp;ROUND(J65,1)&amp;"\\"</f>
+        <f>A7&amp;"&amp;"&amp;'No. vertex and egg'!B5&amp;"&amp;"&amp;'No. vertex and egg'!C5&amp;"&amp;"&amp;IF(C7&lt;=I7,"\bf{"&amp;C7&amp;"}",C7)&amp;"&amp;"&amp;ROUND(D7,1)&amp;"&amp;"&amp;ROUND(E7,1)&amp;"&amp;"&amp;G7&amp;"&amp;"&amp;IF(I7&lt;=C7,"\bf{"&amp;I7&amp;"}",I7)&amp;"&amp;"&amp;ROUND(J7,1)&amp;"&amp;"&amp;IF(C36&lt;=I36,"\bf{"&amp;C36&amp;"}",C36)&amp;"&amp;"&amp;ROUND(D36,1)&amp;"&amp;"&amp;ROUND(E36,1)&amp;"&amp;"&amp;G36&amp;"&amp;"&amp;IF(I36&lt;=C36,"\bf{"&amp;I36&amp;"}",I36)&amp;"&amp;"&amp;ROUND(J36,1)&amp;"&amp;"&amp;IF(C65&lt;=I65,"\bf{"&amp;C65&amp;"}",C65)&amp;"&amp;"&amp;ROUND(D65,1)&amp;"&amp;"&amp;ROUND(E65,1)&amp;"&amp;"&amp;G65&amp;"&amp;"&amp;IF(I65&lt;=C65,"\bf{"&amp;I65&amp;"}",I65)&amp;"&amp;"&amp;ROUND(J65,1)&amp;"\\"</f>
         <v>Bristol&amp;1569&amp;47522&amp;\bf{37}&amp;0&amp;1800.1&amp;BS2&amp;47.4&amp;1&amp;\bf{73.8}&amp;0.4&amp;1800.1&amp;BS4&amp;94&amp;1.4&amp;\bf{146.6}&amp;1.1&amp;1797.8&amp;BS4&amp;176.4&amp;0.8\\</v>
       </c>
     </row>
@@ -777,7 +1970,7 @@
         <v>1</v>
       </c>
       <c r="L8" t="str">
-        <f>A8&amp;"&amp;"&amp;'No. vertex and egg'!B5&amp;"&amp;"&amp;'No. vertex and egg'!C5&amp;"&amp;"&amp;IF(C8&lt;=I8,"\bf{"&amp;C8&amp;"}",C8)&amp;"&amp;"&amp;ROUND(D8,1)&amp;"&amp;"&amp;ROUND(E8,1)&amp;"&amp;"&amp;G8&amp;"&amp;"&amp;IF(I8&lt;=C8,"\bf{"&amp;I8&amp;"}",I8)&amp;"&amp;"&amp;ROUND(J8,1)&amp;"&amp;"&amp;IF(C37&lt;=I37,"\bf{"&amp;C37&amp;"}",C37)&amp;"&amp;"&amp;ROUND(D37,1)&amp;"&amp;"&amp;ROUND(E37,1)&amp;"&amp;"&amp;G37&amp;"&amp;"&amp;IF(I37&lt;=C37,"\bf{"&amp;I37&amp;"}",I37)&amp;"&amp;"&amp;ROUND(J37,1)&amp;"&amp;"&amp;IF(C66&lt;=I66,"\bf{"&amp;C66&amp;"}",C66)&amp;"&amp;"&amp;ROUND(D66,1)&amp;"&amp;"&amp;ROUND(E66,1)&amp;"&amp;"&amp;G66&amp;"&amp;"&amp;IF(I66&lt;=C66,"\bf{"&amp;I66&amp;"}",I66)&amp;"&amp;"&amp;ROUND(J66,1)&amp;"\\"</f>
+        <f>A8&amp;"&amp;"&amp;'No. vertex and egg'!B6&amp;"&amp;"&amp;'No. vertex and egg'!C6&amp;"&amp;"&amp;IF(C8&lt;=I8,"\bf{"&amp;C8&amp;"}",C8)&amp;"&amp;"&amp;ROUND(D8,1)&amp;"&amp;"&amp;ROUND(E8,1)&amp;"&amp;"&amp;G8&amp;"&amp;"&amp;IF(I8&lt;=C8,"\bf{"&amp;I8&amp;"}",I8)&amp;"&amp;"&amp;ROUND(J8,1)&amp;"&amp;"&amp;IF(C37&lt;=I37,"\bf{"&amp;C37&amp;"}",C37)&amp;"&amp;"&amp;ROUND(D37,1)&amp;"&amp;"&amp;ROUND(E37,1)&amp;"&amp;"&amp;G37&amp;"&amp;"&amp;IF(I37&lt;=C37,"\bf{"&amp;I37&amp;"}",I37)&amp;"&amp;"&amp;ROUND(J37,1)&amp;"&amp;"&amp;IF(C66&lt;=I66,"\bf{"&amp;C66&amp;"}",C66)&amp;"&amp;"&amp;ROUND(D66,1)&amp;"&amp;"&amp;ROUND(E66,1)&amp;"&amp;"&amp;G66&amp;"&amp;"&amp;IF(I66&lt;=C66,"\bf{"&amp;I66&amp;"}",I66)&amp;"&amp;"&amp;ROUND(J66,1)&amp;"\\"</f>
         <v>Cardiff&amp;1127&amp;23155&amp;\bf{39}&amp;0&amp;968.2&amp;BS4&amp;50.6&amp;1&amp;\bf{78.3}&amp;0.5&amp;900.5&amp;BS4&amp;95.6&amp;1.6&amp;\bf{157.5}&amp;0.8&amp;660.8&amp;BS4&amp;183.2&amp;1.4\\</v>
       </c>
     </row>
@@ -813,7 +2006,7 @@
         <v>0.4</v>
       </c>
       <c r="L9" t="str">
-        <f>A9&amp;"&amp;"&amp;'No. vertex and egg'!B6&amp;"&amp;"&amp;'No. vertex and egg'!C6&amp;"&amp;"&amp;IF(C9&lt;=I9,"\bf{"&amp;C9&amp;"}",C9)&amp;"&amp;"&amp;ROUND(D9,1)&amp;"&amp;"&amp;ROUND(E9,1)&amp;"&amp;"&amp;G9&amp;"&amp;"&amp;IF(I9&lt;=C9,"\bf{"&amp;I9&amp;"}",I9)&amp;"&amp;"&amp;ROUND(J9,1)&amp;"&amp;"&amp;IF(C38&lt;=I38,"\bf{"&amp;C38&amp;"}",C38)&amp;"&amp;"&amp;ROUND(D38,1)&amp;"&amp;"&amp;ROUND(E38,1)&amp;"&amp;"&amp;G38&amp;"&amp;"&amp;IF(I38&lt;=C38,"\bf{"&amp;I38&amp;"}",I38)&amp;"&amp;"&amp;ROUND(J38,1)&amp;"&amp;"&amp;IF(C67&lt;=I67,"\bf{"&amp;C67&amp;"}",C67)&amp;"&amp;"&amp;ROUND(D67,1)&amp;"&amp;"&amp;ROUND(E67,1)&amp;"&amp;"&amp;G67&amp;"&amp;"&amp;IF(I67&lt;=C67,"\bf{"&amp;I67&amp;"}",I67)&amp;"&amp;"&amp;ROUND(J67,1)&amp;"\\"</f>
+        <f>A9&amp;"&amp;"&amp;'No. vertex and egg'!B7&amp;"&amp;"&amp;'No. vertex and egg'!C7&amp;"&amp;"&amp;IF(C9&lt;=I9,"\bf{"&amp;C9&amp;"}",C9)&amp;"&amp;"&amp;ROUND(D9,1)&amp;"&amp;"&amp;ROUND(E9,1)&amp;"&amp;"&amp;G9&amp;"&amp;"&amp;IF(I9&lt;=C9,"\bf{"&amp;I9&amp;"}",I9)&amp;"&amp;"&amp;ROUND(J9,1)&amp;"&amp;"&amp;IF(C38&lt;=I38,"\bf{"&amp;C38&amp;"}",C38)&amp;"&amp;"&amp;ROUND(D38,1)&amp;"&amp;"&amp;ROUND(E38,1)&amp;"&amp;"&amp;G38&amp;"&amp;"&amp;IF(I38&lt;=C38,"\bf{"&amp;I38&amp;"}",I38)&amp;"&amp;"&amp;ROUND(J38,1)&amp;"&amp;"&amp;IF(C67&lt;=I67,"\bf{"&amp;C67&amp;"}",C67)&amp;"&amp;"&amp;ROUND(D67,1)&amp;"&amp;"&amp;ROUND(E67,1)&amp;"&amp;"&amp;G67&amp;"&amp;"&amp;IF(I67&lt;=C67,"\bf{"&amp;I67&amp;"}",I67)&amp;"&amp;"&amp;ROUND(J67,1)&amp;"\\"</f>
         <v>Coventry&amp;1175&amp;26689&amp;\bf{38}&amp;0&amp;1098.1&amp;BS4&amp;44.8&amp;0.4&amp;\bf{73}&amp;0&amp;1002.5&amp;BS4&amp;85.1&amp;0.7&amp;\bf{149.2}&amp;0.9&amp;827.3&amp;BS4&amp;172.6&amp;1.4\\</v>
       </c>
     </row>
@@ -849,7 +2042,7 @@
         <v>0.5</v>
       </c>
       <c r="L10" t="str">
-        <f>A10&amp;"&amp;"&amp;'No. vertex and egg'!B7&amp;"&amp;"&amp;'No. vertex and egg'!C7&amp;"&amp;"&amp;IF(C10&lt;=I10,"\bf{"&amp;C10&amp;"}",C10)&amp;"&amp;"&amp;ROUND(D10,1)&amp;"&amp;"&amp;ROUND(E10,1)&amp;"&amp;"&amp;G10&amp;"&amp;"&amp;IF(I10&lt;=C10,"\bf{"&amp;I10&amp;"}",I10)&amp;"&amp;"&amp;ROUND(J10,1)&amp;"&amp;"&amp;IF(C39&lt;=I39,"\bf{"&amp;C39&amp;"}",C39)&amp;"&amp;"&amp;ROUND(D39,1)&amp;"&amp;"&amp;ROUND(E39,1)&amp;"&amp;"&amp;G39&amp;"&amp;"&amp;IF(I39&lt;=C39,"\bf{"&amp;I39&amp;"}",I39)&amp;"&amp;"&amp;ROUND(J39,1)&amp;"&amp;"&amp;IF(C68&lt;=I68,"\bf{"&amp;C68&amp;"}",C68)&amp;"&amp;"&amp;ROUND(D68,1)&amp;"&amp;"&amp;ROUND(E68,1)&amp;"&amp;"&amp;G68&amp;"&amp;"&amp;IF(I68&lt;=C68,"\bf{"&amp;I68&amp;"}",I68)&amp;"&amp;"&amp;ROUND(J68,1)&amp;"\\"</f>
+        <f>A10&amp;"&amp;"&amp;'No. vertex and egg'!B8&amp;"&amp;"&amp;'No. vertex and egg'!C8&amp;"&amp;"&amp;IF(C10&lt;=I10,"\bf{"&amp;C10&amp;"}",C10)&amp;"&amp;"&amp;ROUND(D10,1)&amp;"&amp;"&amp;ROUND(E10,1)&amp;"&amp;"&amp;G10&amp;"&amp;"&amp;IF(I10&lt;=C10,"\bf{"&amp;I10&amp;"}",I10)&amp;"&amp;"&amp;ROUND(J10,1)&amp;"&amp;"&amp;IF(C39&lt;=I39,"\bf{"&amp;C39&amp;"}",C39)&amp;"&amp;"&amp;ROUND(D39,1)&amp;"&amp;"&amp;ROUND(E39,1)&amp;"&amp;"&amp;G39&amp;"&amp;"&amp;IF(I39&lt;=C39,"\bf{"&amp;I39&amp;"}",I39)&amp;"&amp;"&amp;ROUND(J39,1)&amp;"&amp;"&amp;IF(C68&lt;=I68,"\bf{"&amp;C68&amp;"}",C68)&amp;"&amp;"&amp;ROUND(D68,1)&amp;"&amp;"&amp;ROUND(E68,1)&amp;"&amp;"&amp;G68&amp;"&amp;"&amp;IF(I68&lt;=C68,"\bf{"&amp;I68&amp;"}",I68)&amp;"&amp;"&amp;ROUND(J68,1)&amp;"\\"</f>
         <v>Exeter&amp;1250&amp;31997&amp;\bf{38}&amp;0&amp;1365.8&amp;BS4&amp;50.6&amp;0.5&amp;\bf{77}&amp;0&amp;1544.2&amp;BS4&amp;95.7&amp;1&amp;\bf{158.1}&amp;0.7&amp;943.2&amp;BS4&amp;182.3&amp;0.6\\</v>
       </c>
     </row>
@@ -885,7 +2078,7 @@
         <v>0.7</v>
       </c>
       <c r="L11" t="str">
-        <f>A11&amp;"&amp;"&amp;'No. vertex and egg'!B8&amp;"&amp;"&amp;'No. vertex and egg'!C8&amp;"&amp;"&amp;IF(C11&lt;=I11,"\bf{"&amp;C11&amp;"}",C11)&amp;"&amp;"&amp;ROUND(D11,1)&amp;"&amp;"&amp;ROUND(E11,1)&amp;"&amp;"&amp;G11&amp;"&amp;"&amp;IF(I11&lt;=C11,"\bf{"&amp;I11&amp;"}",I11)&amp;"&amp;"&amp;ROUND(J11,1)&amp;"&amp;"&amp;IF(C40&lt;=I40,"\bf{"&amp;C40&amp;"}",C40)&amp;"&amp;"&amp;ROUND(D40,1)&amp;"&amp;"&amp;ROUND(E40,1)&amp;"&amp;"&amp;G40&amp;"&amp;"&amp;IF(I40&lt;=C40,"\bf{"&amp;I40&amp;"}",I40)&amp;"&amp;"&amp;ROUND(J40,1)&amp;"&amp;"&amp;IF(C69&lt;=I69,"\bf{"&amp;C69&amp;"}",C69)&amp;"&amp;"&amp;ROUND(D69,1)&amp;"&amp;"&amp;ROUND(E69,1)&amp;"&amp;"&amp;G69&amp;"&amp;"&amp;IF(I69&lt;=C69,"\bf{"&amp;I69&amp;"}",I69)&amp;"&amp;"&amp;ROUND(J69,1)&amp;"\\"</f>
+        <f>A11&amp;"&amp;"&amp;'No. vertex and egg'!B9&amp;"&amp;"&amp;'No. vertex and egg'!C9&amp;"&amp;"&amp;IF(C11&lt;=I11,"\bf{"&amp;C11&amp;"}",C11)&amp;"&amp;"&amp;ROUND(D11,1)&amp;"&amp;"&amp;ROUND(E11,1)&amp;"&amp;"&amp;G11&amp;"&amp;"&amp;IF(I11&lt;=C11,"\bf{"&amp;I11&amp;"}",I11)&amp;"&amp;"&amp;ROUND(J11,1)&amp;"&amp;"&amp;IF(C40&lt;=I40,"\bf{"&amp;C40&amp;"}",C40)&amp;"&amp;"&amp;ROUND(D40,1)&amp;"&amp;"&amp;ROUND(E40,1)&amp;"&amp;"&amp;G40&amp;"&amp;"&amp;IF(I40&lt;=C40,"\bf{"&amp;I40&amp;"}",I40)&amp;"&amp;"&amp;ROUND(J40,1)&amp;"&amp;"&amp;IF(C69&lt;=I69,"\bf{"&amp;C69&amp;"}",C69)&amp;"&amp;"&amp;ROUND(D69,1)&amp;"&amp;"&amp;ROUND(E69,1)&amp;"&amp;"&amp;G69&amp;"&amp;"&amp;IF(I69&lt;=C69,"\bf{"&amp;I69&amp;"}",I69)&amp;"&amp;"&amp;ROUND(J69,1)&amp;"\\"</f>
         <v>Glasgow&amp;1137&amp;24323&amp;\bf{50.1}&amp;0.3&amp;920.6&amp;BS4&amp;59.2&amp;0.7&amp;\bf{94}&amp;0.5&amp;1068.4&amp;BS4&amp;110.6&amp;1.7&amp;\bf{175.2}&amp;0.9&amp;745.6&amp;BS4&amp;199.8&amp;1.6\\</v>
       </c>
     </row>
@@ -921,7 +2114,7 @@
         <v>0.8</v>
       </c>
       <c r="L12" t="str">
-        <f>A12&amp;"&amp;"&amp;'No. vertex and egg'!B9&amp;"&amp;"&amp;'No. vertex and egg'!C9&amp;"&amp;"&amp;IF(C12&lt;=I12,"\bf{"&amp;C12&amp;"}",C12)&amp;"&amp;"&amp;ROUND(D12,1)&amp;"&amp;"&amp;ROUND(E12,1)&amp;"&amp;"&amp;G12&amp;"&amp;"&amp;IF(I12&lt;=C12,"\bf{"&amp;I12&amp;"}",I12)&amp;"&amp;"&amp;ROUND(J12,1)&amp;"&amp;"&amp;IF(C41&lt;=I41,"\bf{"&amp;C41&amp;"}",C41)&amp;"&amp;"&amp;ROUND(D41,1)&amp;"&amp;"&amp;ROUND(E41,1)&amp;"&amp;"&amp;G41&amp;"&amp;"&amp;IF(I41&lt;=C41,"\bf{"&amp;I41&amp;"}",I41)&amp;"&amp;"&amp;ROUND(J41,1)&amp;"&amp;"&amp;IF(C70&lt;=I70,"\bf{"&amp;C70&amp;"}",C70)&amp;"&amp;"&amp;ROUND(D70,1)&amp;"&amp;"&amp;ROUND(E70,1)&amp;"&amp;"&amp;G70&amp;"&amp;"&amp;IF(I70&lt;=C70,"\bf{"&amp;I70&amp;"}",I70)&amp;"&amp;"&amp;ROUND(J70,1)&amp;"\\"</f>
+        <f>A12&amp;"&amp;"&amp;'No. vertex and egg'!B10&amp;"&amp;"&amp;'No. vertex and egg'!C10&amp;"&amp;"&amp;IF(C12&lt;=I12,"\bf{"&amp;C12&amp;"}",C12)&amp;"&amp;"&amp;ROUND(D12,1)&amp;"&amp;"&amp;ROUND(E12,1)&amp;"&amp;"&amp;G12&amp;"&amp;"&amp;IF(I12&lt;=C12,"\bf{"&amp;I12&amp;"}",I12)&amp;"&amp;"&amp;ROUND(J12,1)&amp;"&amp;"&amp;IF(C41&lt;=I41,"\bf{"&amp;C41&amp;"}",C41)&amp;"&amp;"&amp;ROUND(D41,1)&amp;"&amp;"&amp;ROUND(E41,1)&amp;"&amp;"&amp;G41&amp;"&amp;"&amp;IF(I41&lt;=C41,"\bf{"&amp;I41&amp;"}",I41)&amp;"&amp;"&amp;ROUND(J41,1)&amp;"&amp;"&amp;IF(C70&lt;=I70,"\bf{"&amp;C70&amp;"}",C70)&amp;"&amp;"&amp;ROUND(D70,1)&amp;"&amp;"&amp;ROUND(E70,1)&amp;"&amp;"&amp;G70&amp;"&amp;"&amp;IF(I70&lt;=C70,"\bf{"&amp;I70&amp;"}",I70)&amp;"&amp;"&amp;ROUND(J70,1)&amp;"\\"</f>
         <v>Leeds&amp;1647&amp;56511&amp;\bf{40}&amp;0&amp;1800.1&amp;BS4&amp;52.4&amp;0.8&amp;\bf{79.5}&amp;0.5&amp;1800.1&amp;BS4&amp;99.6&amp;1&amp;\bf{152.8}&amp;0.8&amp;1800.1&amp;BS4&amp;187.1&amp;0.7\\</v>
       </c>
     </row>
@@ -957,7 +2150,7 @@
         <v>0.5</v>
       </c>
       <c r="L13" t="str">
-        <f>A13&amp;"&amp;"&amp;'No. vertex and egg'!B10&amp;"&amp;"&amp;'No. vertex and egg'!C10&amp;"&amp;"&amp;IF(C13&lt;=I13,"\bf{"&amp;C13&amp;"}",C13)&amp;"&amp;"&amp;ROUND(D13,1)&amp;"&amp;"&amp;ROUND(E13,1)&amp;"&amp;"&amp;G13&amp;"&amp;"&amp;IF(I13&lt;=C13,"\bf{"&amp;I13&amp;"}",I13)&amp;"&amp;"&amp;ROUND(J13,1)&amp;"&amp;"&amp;IF(C42&lt;=I42,"\bf{"&amp;C42&amp;"}",C42)&amp;"&amp;"&amp;ROUND(D42,1)&amp;"&amp;"&amp;ROUND(E42,1)&amp;"&amp;"&amp;G42&amp;"&amp;"&amp;IF(I42&lt;=C42,"\bf{"&amp;I42&amp;"}",I42)&amp;"&amp;"&amp;ROUND(J42,1)&amp;"&amp;"&amp;IF(C71&lt;=I71,"\bf{"&amp;C71&amp;"}",C71)&amp;"&amp;"&amp;ROUND(D71,1)&amp;"&amp;"&amp;ROUND(E71,1)&amp;"&amp;"&amp;G71&amp;"&amp;"&amp;IF(I71&lt;=C71,"\bf{"&amp;I71&amp;"}",I71)&amp;"&amp;"&amp;ROUND(J71,1)&amp;"\\"</f>
+        <f>A13&amp;"&amp;"&amp;'No. vertex and egg'!B11&amp;"&amp;"&amp;'No. vertex and egg'!C11&amp;"&amp;"&amp;IF(C13&lt;=I13,"\bf{"&amp;C13&amp;"}",C13)&amp;"&amp;"&amp;ROUND(D13,1)&amp;"&amp;"&amp;ROUND(E13,1)&amp;"&amp;"&amp;G13&amp;"&amp;"&amp;IF(I13&lt;=C13,"\bf{"&amp;I13&amp;"}",I13)&amp;"&amp;"&amp;ROUND(J13,1)&amp;"&amp;"&amp;IF(C42&lt;=I42,"\bf{"&amp;C42&amp;"}",C42)&amp;"&amp;"&amp;ROUND(D42,1)&amp;"&amp;"&amp;ROUND(E42,1)&amp;"&amp;"&amp;G42&amp;"&amp;"&amp;IF(I42&lt;=C42,"\bf{"&amp;I42&amp;"}",I42)&amp;"&amp;"&amp;ROUND(J42,1)&amp;"&amp;"&amp;IF(C71&lt;=I71,"\bf{"&amp;C71&amp;"}",C71)&amp;"&amp;"&amp;ROUND(D71,1)&amp;"&amp;"&amp;ROUND(E71,1)&amp;"&amp;"&amp;G71&amp;"&amp;"&amp;IF(I71&lt;=C71,"\bf{"&amp;I71&amp;"}",I71)&amp;"&amp;"&amp;ROUND(J71,1)&amp;"\\"</f>
         <v>Leicester&amp;1531&amp;48219&amp;\bf{38}&amp;0&amp;1800.1&amp;BS4&amp;51.5&amp;0.5&amp;\bf{75}&amp;0&amp;1800.1&amp;BS4&amp;94.1&amp;0.8&amp;\bf{149.3}&amp;0.7&amp;1759&amp;BS4&amp;177.7&amp;1.8\\</v>
       </c>
     </row>
@@ -993,7 +2186,7 @@
         <v>0.5</v>
       </c>
       <c r="L14" t="str">
-        <f>A14&amp;"&amp;"&amp;'No. vertex and egg'!B11&amp;"&amp;"&amp;'No. vertex and egg'!C11&amp;"&amp;"&amp;IF(C14&lt;=I14,"\bf{"&amp;C14&amp;"}",C14)&amp;"&amp;"&amp;ROUND(D14,1)&amp;"&amp;"&amp;ROUND(E14,1)&amp;"&amp;"&amp;G14&amp;"&amp;"&amp;IF(I14&lt;=C14,"\bf{"&amp;I14&amp;"}",I14)&amp;"&amp;"&amp;ROUND(J14,1)&amp;"&amp;"&amp;IF(C43&lt;=I43,"\bf{"&amp;C43&amp;"}",C43)&amp;"&amp;"&amp;ROUND(D43,1)&amp;"&amp;"&amp;ROUND(E43,1)&amp;"&amp;"&amp;G43&amp;"&amp;"&amp;IF(I43&lt;=C43,"\bf{"&amp;I43&amp;"}",I43)&amp;"&amp;"&amp;ROUND(J43,1)&amp;"&amp;"&amp;IF(C72&lt;=I72,"\bf{"&amp;C72&amp;"}",C72)&amp;"&amp;"&amp;ROUND(D72,1)&amp;"&amp;"&amp;ROUND(E72,1)&amp;"&amp;"&amp;G72&amp;"&amp;"&amp;IF(I72&lt;=C72,"\bf{"&amp;I72&amp;"}",I72)&amp;"&amp;"&amp;ROUND(J72,1)&amp;"\\"</f>
+        <f>A14&amp;"&amp;"&amp;'No. vertex and egg'!B12&amp;"&amp;"&amp;'No. vertex and egg'!C12&amp;"&amp;"&amp;IF(C14&lt;=I14,"\bf{"&amp;C14&amp;"}",C14)&amp;"&amp;"&amp;ROUND(D14,1)&amp;"&amp;"&amp;ROUND(E14,1)&amp;"&amp;"&amp;G14&amp;"&amp;"&amp;IF(I14&lt;=C14,"\bf{"&amp;I14&amp;"}",I14)&amp;"&amp;"&amp;ROUND(J14,1)&amp;"&amp;"&amp;IF(C43&lt;=I43,"\bf{"&amp;C43&amp;"}",C43)&amp;"&amp;"&amp;ROUND(D43,1)&amp;"&amp;"&amp;ROUND(E43,1)&amp;"&amp;"&amp;G43&amp;"&amp;"&amp;IF(I43&lt;=C43,"\bf{"&amp;I43&amp;"}",I43)&amp;"&amp;"&amp;ROUND(J43,1)&amp;"&amp;"&amp;IF(C72&lt;=I72,"\bf{"&amp;C72&amp;"}",C72)&amp;"&amp;"&amp;ROUND(D72,1)&amp;"&amp;"&amp;ROUND(E72,1)&amp;"&amp;"&amp;G72&amp;"&amp;"&amp;IF(I72&lt;=C72,"\bf{"&amp;I72&amp;"}",I72)&amp;"&amp;"&amp;ROUND(J72,1)&amp;"\\"</f>
         <v>Liverpool&amp;1273&amp;42564&amp;\bf{28}&amp;0&amp;1800.1&amp;BS4&amp;38.4&amp;0.5&amp;\bf{57}&amp;0.5&amp;1800.1&amp;BS4&amp;72&amp;0.8&amp;\bf{112.8}&amp;0.6&amp;1800.1&amp;BS4&amp;133&amp;0.8\\</v>
       </c>
     </row>
@@ -1029,7 +2222,7 @@
         <v>0.5</v>
       </c>
       <c r="L15" t="str">
-        <f>A15&amp;"&amp;"&amp;'No. vertex and egg'!B12&amp;"&amp;"&amp;'No. vertex and egg'!C12&amp;"&amp;"&amp;IF(C15&lt;=I15,"\bf{"&amp;C15&amp;"}",C15)&amp;"&amp;"&amp;ROUND(D15,1)&amp;"&amp;"&amp;ROUND(E15,1)&amp;"&amp;"&amp;G15&amp;"&amp;"&amp;IF(I15&lt;=C15,"\bf{"&amp;I15&amp;"}",I15)&amp;"&amp;"&amp;ROUND(J15,1)&amp;"&amp;"&amp;IF(C44&lt;=I44,"\bf{"&amp;C44&amp;"}",C44)&amp;"&amp;"&amp;ROUND(D44,1)&amp;"&amp;"&amp;ROUND(E44,1)&amp;"&amp;"&amp;G44&amp;"&amp;"&amp;IF(I44&lt;=C44,"\bf{"&amp;I44&amp;"}",I44)&amp;"&amp;"&amp;ROUND(J44,1)&amp;"&amp;"&amp;IF(C73&lt;=I73,"\bf{"&amp;C73&amp;"}",C73)&amp;"&amp;"&amp;ROUND(D73,1)&amp;"&amp;"&amp;ROUND(E73,1)&amp;"&amp;"&amp;G73&amp;"&amp;"&amp;IF(I73&lt;=C73,"\bf{"&amp;I73&amp;"}",I73)&amp;"&amp;"&amp;ROUND(J73,1)&amp;"\\"</f>
+        <f>A15&amp;"&amp;"&amp;'No. vertex and egg'!B13&amp;"&amp;"&amp;'No. vertex and egg'!C13&amp;"&amp;"&amp;IF(C15&lt;=I15,"\bf{"&amp;C15&amp;"}",C15)&amp;"&amp;"&amp;ROUND(D15,1)&amp;"&amp;"&amp;ROUND(E15,1)&amp;"&amp;"&amp;G15&amp;"&amp;"&amp;IF(I15&lt;=C15,"\bf{"&amp;I15&amp;"}",I15)&amp;"&amp;"&amp;ROUND(J15,1)&amp;"&amp;"&amp;IF(C44&lt;=I44,"\bf{"&amp;C44&amp;"}",C44)&amp;"&amp;"&amp;ROUND(D44,1)&amp;"&amp;"&amp;ROUND(E44,1)&amp;"&amp;"&amp;G44&amp;"&amp;"&amp;IF(I44&lt;=C44,"\bf{"&amp;I44&amp;"}",I44)&amp;"&amp;"&amp;ROUND(J44,1)&amp;"&amp;"&amp;IF(C73&lt;=I73,"\bf{"&amp;C73&amp;"}",C73)&amp;"&amp;"&amp;ROUND(D73,1)&amp;"&amp;"&amp;ROUND(E73,1)&amp;"&amp;"&amp;G73&amp;"&amp;"&amp;IF(I73&lt;=C73,"\bf{"&amp;I73&amp;"}",I73)&amp;"&amp;"&amp;ROUND(J73,1)&amp;"\\"</f>
         <v>Manchester&amp;1991&amp;77286&amp;\bf{38.3}&amp;0.7&amp;1800.2&amp;BS4&amp;45.9&amp;0.5&amp;\bf{77.9}&amp;0.3&amp;1800.1&amp;BS4&amp;91.5&amp;0.9&amp;\bf{155.2}&amp;0.6&amp;1800.1&amp;BS4&amp;178.5&amp;1\\</v>
       </c>
     </row>
@@ -1065,7 +2258,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="L16" t="str">
-        <f>A16&amp;"&amp;"&amp;'No. vertex and egg'!B13&amp;"&amp;"&amp;'No. vertex and egg'!C13&amp;"&amp;"&amp;IF(C16&lt;=I16,"\bf{"&amp;C16&amp;"}",C16)&amp;"&amp;"&amp;ROUND(D16,1)&amp;"&amp;"&amp;ROUND(E16,1)&amp;"&amp;"&amp;G16&amp;"&amp;"&amp;IF(I16&lt;=C16,"\bf{"&amp;I16&amp;"}",I16)&amp;"&amp;"&amp;ROUND(J16,1)&amp;"&amp;"&amp;IF(C45&lt;=I45,"\bf{"&amp;C45&amp;"}",C45)&amp;"&amp;"&amp;ROUND(D45,1)&amp;"&amp;"&amp;ROUND(E45,1)&amp;"&amp;"&amp;G45&amp;"&amp;"&amp;IF(I45&lt;=C45,"\bf{"&amp;I45&amp;"}",I45)&amp;"&amp;"&amp;ROUND(J45,1)&amp;"&amp;"&amp;IF(C74&lt;=I74,"\bf{"&amp;C74&amp;"}",C74)&amp;"&amp;"&amp;ROUND(D74,1)&amp;"&amp;"&amp;ROUND(E74,1)&amp;"&amp;"&amp;G74&amp;"&amp;"&amp;IF(I74&lt;=C74,"\bf{"&amp;I74&amp;"}",I74)&amp;"&amp;"&amp;ROUND(J74,1)&amp;"\\"</f>
+        <f>A16&amp;"&amp;"&amp;'No. vertex and egg'!B14&amp;"&amp;"&amp;'No. vertex and egg'!C14&amp;"&amp;"&amp;IF(C16&lt;=I16,"\bf{"&amp;C16&amp;"}",C16)&amp;"&amp;"&amp;ROUND(D16,1)&amp;"&amp;"&amp;ROUND(E16,1)&amp;"&amp;"&amp;G16&amp;"&amp;"&amp;IF(I16&lt;=C16,"\bf{"&amp;I16&amp;"}",I16)&amp;"&amp;"&amp;ROUND(J16,1)&amp;"&amp;"&amp;IF(C45&lt;=I45,"\bf{"&amp;C45&amp;"}",C45)&amp;"&amp;"&amp;ROUND(D45,1)&amp;"&amp;"&amp;ROUND(E45,1)&amp;"&amp;"&amp;G45&amp;"&amp;"&amp;IF(I45&lt;=C45,"\bf{"&amp;I45&amp;"}",I45)&amp;"&amp;"&amp;ROUND(J45,1)&amp;"&amp;"&amp;IF(C74&lt;=I74,"\bf{"&amp;C74&amp;"}",C74)&amp;"&amp;"&amp;ROUND(D74,1)&amp;"&amp;"&amp;ROUND(E74,1)&amp;"&amp;"&amp;G74&amp;"&amp;"&amp;IF(I74&lt;=C74,"\bf{"&amp;I74&amp;"}",I74)&amp;"&amp;"&amp;ROUND(J74,1)&amp;"\\"</f>
         <v>Newcastle&amp;1109&amp;26614&amp;\bf{44}&amp;0&amp;1146.4&amp;BS4&amp;52.6&amp;1.1&amp;\bf{83.6}&amp;0.5&amp;1020.5&amp;BS4&amp;95.4&amp;1.1&amp;\bf{152.4}&amp;0.5&amp;951.3&amp;BS2&amp;171.5&amp;1.2\\</v>
       </c>
     </row>
@@ -1101,7 +2294,7 @@
         <v>0.8</v>
       </c>
       <c r="L17" t="str">
-        <f>A17&amp;"&amp;"&amp;'No. vertex and egg'!B14&amp;"&amp;"&amp;'No. vertex and egg'!C14&amp;"&amp;"&amp;IF(C17&lt;=I17,"\bf{"&amp;C17&amp;"}",C17)&amp;"&amp;"&amp;ROUND(D17,1)&amp;"&amp;"&amp;ROUND(E17,1)&amp;"&amp;"&amp;G17&amp;"&amp;"&amp;IF(I17&lt;=C17,"\bf{"&amp;I17&amp;"}",I17)&amp;"&amp;"&amp;ROUND(J17,1)&amp;"&amp;"&amp;IF(C46&lt;=I46,"\bf{"&amp;C46&amp;"}",C46)&amp;"&amp;"&amp;ROUND(D46,1)&amp;"&amp;"&amp;ROUND(E46,1)&amp;"&amp;"&amp;G46&amp;"&amp;"&amp;IF(I46&lt;=C46,"\bf{"&amp;I46&amp;"}",I46)&amp;"&amp;"&amp;ROUND(J46,1)&amp;"&amp;"&amp;IF(C75&lt;=I75,"\bf{"&amp;C75&amp;"}",C75)&amp;"&amp;"&amp;ROUND(D75,1)&amp;"&amp;"&amp;ROUND(E75,1)&amp;"&amp;"&amp;G75&amp;"&amp;"&amp;IF(I75&lt;=C75,"\bf{"&amp;I75&amp;"}",I75)&amp;"&amp;"&amp;ROUND(J75,1)&amp;"\\"</f>
+        <f>A17&amp;"&amp;"&amp;'No. vertex and egg'!B15&amp;"&amp;"&amp;'No. vertex and egg'!C15&amp;"&amp;"&amp;IF(C17&lt;=I17,"\bf{"&amp;C17&amp;"}",C17)&amp;"&amp;"&amp;ROUND(D17,1)&amp;"&amp;"&amp;ROUND(E17,1)&amp;"&amp;"&amp;G17&amp;"&amp;"&amp;IF(I17&lt;=C17,"\bf{"&amp;I17&amp;"}",I17)&amp;"&amp;"&amp;ROUND(J17,1)&amp;"&amp;"&amp;IF(C46&lt;=I46,"\bf{"&amp;C46&amp;"}",C46)&amp;"&amp;"&amp;ROUND(D46,1)&amp;"&amp;"&amp;ROUND(E46,1)&amp;"&amp;"&amp;G46&amp;"&amp;"&amp;IF(I46&lt;=C46,"\bf{"&amp;I46&amp;"}",I46)&amp;"&amp;"&amp;ROUND(J46,1)&amp;"&amp;"&amp;IF(C75&lt;=I75,"\bf{"&amp;C75&amp;"}",C75)&amp;"&amp;"&amp;ROUND(D75,1)&amp;"&amp;"&amp;ROUND(E75,1)&amp;"&amp;"&amp;G75&amp;"&amp;"&amp;IF(I75&lt;=C75,"\bf{"&amp;I75&amp;"}",I75)&amp;"&amp;"&amp;ROUND(J75,1)&amp;"\\"</f>
         <v>Nottingham&amp;1739&amp;51595&amp;\bf{44}&amp;0&amp;1799.1&amp;BS4&amp;56.6&amp;0.8&amp;\bf{84.7}&amp;0.5&amp;1800.2&amp;BS4&amp;103.3&amp;0.8&amp;\bf{164.2}&amp;0.8&amp;1800.2&amp;BS4&amp;195.2&amp;1.2\\</v>
       </c>
     </row>
@@ -1137,7 +2330,7 @@
         <v>0.5</v>
       </c>
       <c r="L18" t="str">
-        <f>A18&amp;"&amp;"&amp;'No. vertex and egg'!B15&amp;"&amp;"&amp;'No. vertex and egg'!C15&amp;"&amp;"&amp;IF(C18&lt;=I18,"\bf{"&amp;C18&amp;"}",C18)&amp;"&amp;"&amp;ROUND(D18,1)&amp;"&amp;"&amp;ROUND(E18,1)&amp;"&amp;"&amp;G18&amp;"&amp;"&amp;IF(I18&lt;=C18,"\bf{"&amp;I18&amp;"}",I18)&amp;"&amp;"&amp;ROUND(J18,1)&amp;"&amp;"&amp;IF(C47&lt;=I47,"\bf{"&amp;C47&amp;"}",C47)&amp;"&amp;"&amp;ROUND(D47,1)&amp;"&amp;"&amp;ROUND(E47,1)&amp;"&amp;"&amp;G47&amp;"&amp;"&amp;IF(I47&lt;=C47,"\bf{"&amp;I47&amp;"}",I47)&amp;"&amp;"&amp;ROUND(J47,1)&amp;"&amp;"&amp;IF(C76&lt;=I76,"\bf{"&amp;C76&amp;"}",C76)&amp;"&amp;"&amp;ROUND(D76,1)&amp;"&amp;"&amp;ROUND(E76,1)&amp;"&amp;"&amp;G76&amp;"&amp;"&amp;IF(I76&lt;=C76,"\bf{"&amp;I76&amp;"}",I76)&amp;"&amp;"&amp;ROUND(J76,1)&amp;"\\"</f>
+        <f>A18&amp;"&amp;"&amp;'No. vertex and egg'!B16&amp;"&amp;"&amp;'No. vertex and egg'!C16&amp;"&amp;"&amp;IF(C18&lt;=I18,"\bf{"&amp;C18&amp;"}",C18)&amp;"&amp;"&amp;ROUND(D18,1)&amp;"&amp;"&amp;ROUND(E18,1)&amp;"&amp;"&amp;G18&amp;"&amp;"&amp;IF(I18&lt;=C18,"\bf{"&amp;I18&amp;"}",I18)&amp;"&amp;"&amp;ROUND(J18,1)&amp;"&amp;"&amp;IF(C47&lt;=I47,"\bf{"&amp;C47&amp;"}",C47)&amp;"&amp;"&amp;ROUND(D47,1)&amp;"&amp;"&amp;ROUND(E47,1)&amp;"&amp;"&amp;G47&amp;"&amp;"&amp;IF(I47&lt;=C47,"\bf{"&amp;I47&amp;"}",I47)&amp;"&amp;"&amp;ROUND(J47,1)&amp;"&amp;"&amp;IF(C76&lt;=I76,"\bf{"&amp;C76&amp;"}",C76)&amp;"&amp;"&amp;ROUND(D76,1)&amp;"&amp;"&amp;ROUND(E76,1)&amp;"&amp;"&amp;G76&amp;"&amp;"&amp;IF(I76&lt;=C76,"\bf{"&amp;I76&amp;"}",I76)&amp;"&amp;"&amp;ROUND(J76,1)&amp;"\\"</f>
         <v>Oxford&amp;479&amp;8396&amp;\bf{24}&amp;0&amp;263.1&amp;BS4&amp;27.9&amp;0.5&amp;\bf{47}&amp;0&amp;298&amp;BS4&amp;54.9&amp;0.7&amp;\bf{89}&amp;0&amp;254.4&amp;BS2&amp;100.8&amp;0.9\\</v>
       </c>
     </row>
@@ -1173,7 +2366,7 @@
         <v>0.8</v>
       </c>
       <c r="L19" t="str">
-        <f>A19&amp;"&amp;"&amp;'No. vertex and egg'!B16&amp;"&amp;"&amp;'No. vertex and egg'!C16&amp;"&amp;"&amp;IF(C19&lt;=I19,"\bf{"&amp;C19&amp;"}",C19)&amp;"&amp;"&amp;ROUND(D19,1)&amp;"&amp;"&amp;ROUND(E19,1)&amp;"&amp;"&amp;G19&amp;"&amp;"&amp;IF(I19&lt;=C19,"\bf{"&amp;I19&amp;"}",I19)&amp;"&amp;"&amp;ROUND(J19,1)&amp;"&amp;"&amp;IF(C48&lt;=I48,"\bf{"&amp;C48&amp;"}",C48)&amp;"&amp;"&amp;ROUND(D48,1)&amp;"&amp;"&amp;ROUND(E48,1)&amp;"&amp;"&amp;G48&amp;"&amp;"&amp;IF(I48&lt;=C48,"\bf{"&amp;I48&amp;"}",I48)&amp;"&amp;"&amp;ROUND(J48,1)&amp;"&amp;"&amp;IF(C77&lt;=I77,"\bf{"&amp;C77&amp;"}",C77)&amp;"&amp;"&amp;ROUND(D77,1)&amp;"&amp;"&amp;ROUND(E77,1)&amp;"&amp;"&amp;G77&amp;"&amp;"&amp;IF(I77&lt;=C77,"\bf{"&amp;I77&amp;"}",I77)&amp;"&amp;"&amp;ROUND(J77,1)&amp;"\\"</f>
+        <f>A19&amp;"&amp;"&amp;'No. vertex and egg'!B17&amp;"&amp;"&amp;'No. vertex and egg'!C17&amp;"&amp;"&amp;IF(C19&lt;=I19,"\bf{"&amp;C19&amp;"}",C19)&amp;"&amp;"&amp;ROUND(D19,1)&amp;"&amp;"&amp;ROUND(E19,1)&amp;"&amp;"&amp;G19&amp;"&amp;"&amp;IF(I19&lt;=C19,"\bf{"&amp;I19&amp;"}",I19)&amp;"&amp;"&amp;ROUND(J19,1)&amp;"&amp;"&amp;IF(C48&lt;=I48,"\bf{"&amp;C48&amp;"}",C48)&amp;"&amp;"&amp;ROUND(D48,1)&amp;"&amp;"&amp;ROUND(E48,1)&amp;"&amp;"&amp;G48&amp;"&amp;"&amp;IF(I48&lt;=C48,"\bf{"&amp;I48&amp;"}",I48)&amp;"&amp;"&amp;ROUND(J48,1)&amp;"&amp;"&amp;IF(C77&lt;=I77,"\bf{"&amp;C77&amp;"}",C77)&amp;"&amp;"&amp;ROUND(D77,1)&amp;"&amp;"&amp;ROUND(E77,1)&amp;"&amp;"&amp;G77&amp;"&amp;"&amp;IF(I77&lt;=C77,"\bf{"&amp;I77&amp;"}",I77)&amp;"&amp;"&amp;ROUND(J77,1)&amp;"\\"</f>
         <v>Plymouth&amp;1122&amp;35070&amp;\bf{31}&amp;0&amp;1398.8&amp;BS4&amp;40.3&amp;0.8&amp;\bf{61.3}&amp;0.5&amp;1694.2&amp;BS4&amp;75&amp;1.1&amp;\bf{115.6}&amp;0.5&amp;1688&amp;BS4&amp;137&amp;1.2\\</v>
       </c>
     </row>
@@ -1209,7 +2402,7 @@
         <v>0.7</v>
       </c>
       <c r="L20" t="str">
-        <f>A20&amp;"&amp;"&amp;'No. vertex and egg'!B17&amp;"&amp;"&amp;'No. vertex and egg'!C17&amp;"&amp;"&amp;IF(C20&lt;=I20,"\bf{"&amp;C20&amp;"}",C20)&amp;"&amp;"&amp;ROUND(D20,1)&amp;"&amp;"&amp;ROUND(E20,1)&amp;"&amp;"&amp;G20&amp;"&amp;"&amp;IF(I20&lt;=C20,"\bf{"&amp;I20&amp;"}",I20)&amp;"&amp;"&amp;ROUND(J20,1)&amp;"&amp;"&amp;IF(C49&lt;=I49,"\bf{"&amp;C49&amp;"}",C49)&amp;"&amp;"&amp;ROUND(D49,1)&amp;"&amp;"&amp;ROUND(E49,1)&amp;"&amp;"&amp;G49&amp;"&amp;"&amp;IF(I49&lt;=C49,"\bf{"&amp;I49&amp;"}",I49)&amp;"&amp;"&amp;ROUND(J49,1)&amp;"&amp;"&amp;IF(C78&lt;=I78,"\bf{"&amp;C78&amp;"}",C78)&amp;"&amp;"&amp;ROUND(D78,1)&amp;"&amp;"&amp;ROUND(E78,1)&amp;"&amp;"&amp;G78&amp;"&amp;"&amp;IF(I78&lt;=C78,"\bf{"&amp;I78&amp;"}",I78)&amp;"&amp;"&amp;ROUND(J78,1)&amp;"\\"</f>
+        <f>A20&amp;"&amp;"&amp;'No. vertex and egg'!B18&amp;"&amp;"&amp;'No. vertex and egg'!C18&amp;"&amp;"&amp;IF(C20&lt;=I20,"\bf{"&amp;C20&amp;"}",C20)&amp;"&amp;"&amp;ROUND(D20,1)&amp;"&amp;"&amp;ROUND(E20,1)&amp;"&amp;"&amp;G20&amp;"&amp;"&amp;IF(I20&lt;=C20,"\bf{"&amp;I20&amp;"}",I20)&amp;"&amp;"&amp;ROUND(J20,1)&amp;"&amp;"&amp;IF(C49&lt;=I49,"\bf{"&amp;C49&amp;"}",C49)&amp;"&amp;"&amp;ROUND(D49,1)&amp;"&amp;"&amp;ROUND(E49,1)&amp;"&amp;"&amp;G49&amp;"&amp;"&amp;IF(I49&lt;=C49,"\bf{"&amp;I49&amp;"}",I49)&amp;"&amp;"&amp;ROUND(J49,1)&amp;"&amp;"&amp;IF(C78&lt;=I78,"\bf{"&amp;C78&amp;"}",C78)&amp;"&amp;"&amp;ROUND(D78,1)&amp;"&amp;"&amp;ROUND(E78,1)&amp;"&amp;"&amp;G78&amp;"&amp;"&amp;IF(I78&lt;=C78,"\bf{"&amp;I78&amp;"}",I78)&amp;"&amp;"&amp;ROUND(J78,1)&amp;"\\"</f>
         <v>Sheffield&amp;1582&amp;50534&amp;\bf{42}&amp;0&amp;1800.2&amp;BS4&amp;52.5&amp;0.7&amp;\bf{84.6}&amp;0.5&amp;1747.7&amp;BS4&amp;98.9&amp;1.3&amp;\bf{161.4}&amp;0.8&amp;1800&amp;BS4&amp;182.2&amp;1.2\\</v>
       </c>
     </row>
@@ -1245,7 +2438,7 @@
         <v>0.8</v>
       </c>
       <c r="L21" t="str">
-        <f>A21&amp;"&amp;"&amp;'No. vertex and egg'!B18&amp;"&amp;"&amp;'No. vertex and egg'!C18&amp;"&amp;"&amp;IF(C21&lt;=I21,"\bf{"&amp;C21&amp;"}",C21)&amp;"&amp;"&amp;ROUND(D21,1)&amp;"&amp;"&amp;ROUND(E21,1)&amp;"&amp;"&amp;G21&amp;"&amp;"&amp;IF(I21&lt;=C21,"\bf{"&amp;I21&amp;"}",I21)&amp;"&amp;"&amp;ROUND(J21,1)&amp;"&amp;"&amp;IF(C50&lt;=I50,"\bf{"&amp;C50&amp;"}",C50)&amp;"&amp;"&amp;ROUND(D50,1)&amp;"&amp;"&amp;ROUND(E50,1)&amp;"&amp;"&amp;G50&amp;"&amp;"&amp;IF(I50&lt;=C50,"\bf{"&amp;I50&amp;"}",I50)&amp;"&amp;"&amp;ROUND(J50,1)&amp;"&amp;"&amp;IF(C79&lt;=I79,"\bf{"&amp;C79&amp;"}",C79)&amp;"&amp;"&amp;ROUND(D79,1)&amp;"&amp;"&amp;ROUND(E79,1)&amp;"&amp;"&amp;G79&amp;"&amp;"&amp;IF(I79&lt;=C79,"\bf{"&amp;I79&amp;"}",I79)&amp;"&amp;"&amp;ROUND(J79,1)&amp;"\\"</f>
+        <f>A21&amp;"&amp;"&amp;'No. vertex and egg'!B19&amp;"&amp;"&amp;'No. vertex and egg'!C19&amp;"&amp;"&amp;IF(C21&lt;=I21,"\bf{"&amp;C21&amp;"}",C21)&amp;"&amp;"&amp;ROUND(D21,1)&amp;"&amp;"&amp;ROUND(E21,1)&amp;"&amp;"&amp;G21&amp;"&amp;"&amp;IF(I21&lt;=C21,"\bf{"&amp;I21&amp;"}",I21)&amp;"&amp;"&amp;ROUND(J21,1)&amp;"&amp;"&amp;IF(C50&lt;=I50,"\bf{"&amp;C50&amp;"}",C50)&amp;"&amp;"&amp;ROUND(D50,1)&amp;"&amp;"&amp;ROUND(E50,1)&amp;"&amp;"&amp;G50&amp;"&amp;"&amp;IF(I50&lt;=C50,"\bf{"&amp;I50&amp;"}",I50)&amp;"&amp;"&amp;ROUND(J50,1)&amp;"&amp;"&amp;IF(C79&lt;=I79,"\bf{"&amp;C79&amp;"}",C79)&amp;"&amp;"&amp;ROUND(D79,1)&amp;"&amp;"&amp;ROUND(E79,1)&amp;"&amp;"&amp;G79&amp;"&amp;"&amp;IF(I79&lt;=C79,"\bf{"&amp;I79&amp;"}",I79)&amp;"&amp;"&amp;ROUND(J79,1)&amp;"\\"</f>
         <v>Southampton&amp;796&amp;19942&amp;\bf{25}&amp;0&amp;750.1&amp;BS4&amp;29.6&amp;0.8&amp;\bf{49.2}&amp;0.4&amp;807.2&amp;BS4&amp;61.1&amp;0.7&amp;\bf{97.6}&amp;0.5&amp;1129&amp;BS4&amp;113.2&amp;1.4\\</v>
       </c>
     </row>
@@ -1281,7 +2474,7 @@
         <v>0.4</v>
       </c>
       <c r="L22" t="str">
-        <f>A22&amp;"&amp;"&amp;'No. vertex and egg'!B19&amp;"&amp;"&amp;'No. vertex and egg'!C19&amp;"&amp;"&amp;IF(C22&lt;=I22,"\bf{"&amp;C22&amp;"}",C22)&amp;"&amp;"&amp;ROUND(D22,1)&amp;"&amp;"&amp;ROUND(E22,1)&amp;"&amp;"&amp;G22&amp;"&amp;"&amp;IF(I22&lt;=C22,"\bf{"&amp;I22&amp;"}",I22)&amp;"&amp;"&amp;ROUND(J22,1)&amp;"&amp;"&amp;IF(C51&lt;=I51,"\bf{"&amp;C51&amp;"}",C51)&amp;"&amp;"&amp;ROUND(D51,1)&amp;"&amp;"&amp;ROUND(E51,1)&amp;"&amp;"&amp;G51&amp;"&amp;"&amp;IF(I51&lt;=C51,"\bf{"&amp;I51&amp;"}",I51)&amp;"&amp;"&amp;ROUND(J51,1)&amp;"&amp;"&amp;IF(C80&lt;=I80,"\bf{"&amp;C80&amp;"}",C80)&amp;"&amp;"&amp;ROUND(D80,1)&amp;"&amp;"&amp;ROUND(E80,1)&amp;"&amp;"&amp;G80&amp;"&amp;"&amp;IF(I80&lt;=C80,"\bf{"&amp;I80&amp;"}",I80)&amp;"&amp;"&amp;ROUND(J80,1)&amp;"\\"</f>
+        <f>A22&amp;"&amp;"&amp;'No. vertex and egg'!B20&amp;"&amp;"&amp;'No. vertex and egg'!C20&amp;"&amp;"&amp;IF(C22&lt;=I22,"\bf{"&amp;C22&amp;"}",C22)&amp;"&amp;"&amp;ROUND(D22,1)&amp;"&amp;"&amp;ROUND(E22,1)&amp;"&amp;"&amp;G22&amp;"&amp;"&amp;IF(I22&lt;=C22,"\bf{"&amp;I22&amp;"}",I22)&amp;"&amp;"&amp;ROUND(J22,1)&amp;"&amp;"&amp;IF(C51&lt;=I51,"\bf{"&amp;C51&amp;"}",C51)&amp;"&amp;"&amp;ROUND(D51,1)&amp;"&amp;"&amp;ROUND(E51,1)&amp;"&amp;"&amp;G51&amp;"&amp;"&amp;IF(I51&lt;=C51,"\bf{"&amp;I51&amp;"}",I51)&amp;"&amp;"&amp;ROUND(J51,1)&amp;"&amp;"&amp;IF(C80&lt;=I80,"\bf{"&amp;C80&amp;"}",C80)&amp;"&amp;"&amp;ROUND(D80,1)&amp;"&amp;"&amp;ROUND(E80,1)&amp;"&amp;"&amp;G80&amp;"&amp;"&amp;IF(I80&lt;=C80,"\bf{"&amp;I80&amp;"}",I80)&amp;"&amp;"&amp;ROUND(J80,1)&amp;"\\"</f>
         <v>Sunderland&amp;1346&amp;42013&amp;\bf{36}&amp;0&amp;1559.3&amp;BS4&amp;46.3&amp;0.4&amp;\bf{73}&amp;0&amp;1049&amp;BS4&amp;89.1&amp;1.1&amp;\bf{141}&amp;0.5&amp;1438.3&amp;BS4&amp;163.6&amp;1\\</v>
       </c>
     </row>
@@ -1317,7 +2510,7 @@
         <v>0.3</v>
       </c>
       <c r="L23" t="str">
-        <f>A23&amp;"&amp;"&amp;'No. vertex and egg'!B20&amp;"&amp;"&amp;'No. vertex and egg'!C20&amp;"&amp;"&amp;IF(C23&lt;=I23,"\bf{"&amp;C23&amp;"}",C23)&amp;"&amp;"&amp;ROUND(D23,1)&amp;"&amp;"&amp;ROUND(E23,1)&amp;"&amp;"&amp;G23&amp;"&amp;"&amp;IF(I23&lt;=C23,"\bf{"&amp;I23&amp;"}",I23)&amp;"&amp;"&amp;ROUND(J23,1)&amp;"&amp;"&amp;IF(C52&lt;=I52,"\bf{"&amp;C52&amp;"}",C52)&amp;"&amp;"&amp;ROUND(D52,1)&amp;"&amp;"&amp;ROUND(E52,1)&amp;"&amp;"&amp;G52&amp;"&amp;"&amp;IF(I52&lt;=C52,"\bf{"&amp;I52&amp;"}",I52)&amp;"&amp;"&amp;ROUND(J52,1)&amp;"&amp;"&amp;IF(C81&lt;=I81,"\bf{"&amp;C81&amp;"}",C81)&amp;"&amp;"&amp;ROUND(D81,1)&amp;"&amp;"&amp;ROUND(E81,1)&amp;"&amp;"&amp;G81&amp;"&amp;"&amp;IF(I81&lt;=C81,"\bf{"&amp;I81&amp;"}",I81)&amp;"&amp;"&amp;ROUND(J81,1)&amp;"\\"</f>
+        <f>A23&amp;"&amp;"&amp;'No. vertex and egg'!B21&amp;"&amp;"&amp;'No. vertex and egg'!C21&amp;"&amp;"&amp;IF(C23&lt;=I23,"\bf{"&amp;C23&amp;"}",C23)&amp;"&amp;"&amp;ROUND(D23,1)&amp;"&amp;"&amp;ROUND(E23,1)&amp;"&amp;"&amp;G23&amp;"&amp;"&amp;IF(I23&lt;=C23,"\bf{"&amp;I23&amp;"}",I23)&amp;"&amp;"&amp;ROUND(J23,1)&amp;"&amp;"&amp;IF(C52&lt;=I52,"\bf{"&amp;C52&amp;"}",C52)&amp;"&amp;"&amp;ROUND(D52,1)&amp;"&amp;"&amp;ROUND(E52,1)&amp;"&amp;"&amp;G52&amp;"&amp;"&amp;IF(I52&lt;=C52,"\bf{"&amp;I52&amp;"}",I52)&amp;"&amp;"&amp;ROUND(J52,1)&amp;"&amp;"&amp;IF(C81&lt;=I81,"\bf{"&amp;C81&amp;"}",C81)&amp;"&amp;"&amp;ROUND(D81,1)&amp;"&amp;"&amp;ROUND(E81,1)&amp;"&amp;"&amp;G81&amp;"&amp;"&amp;IF(I81&lt;=C81,"\bf{"&amp;I81&amp;"}",I81)&amp;"&amp;"&amp;ROUND(J81,1)&amp;"\\"</f>
         <v>York&amp;1044&amp;23774&amp;\bf{32}&amp;0&amp;856.8&amp;BS4&amp;39.1&amp;0.3&amp;\bf{68}&amp;0&amp;573&amp;BS4&amp;77.6&amp;0.6&amp;\bf{130.4}&amp;0.5&amp;784.5&amp;BS4&amp;145.8&amp;1.2\\</v>
       </c>
     </row>
@@ -1353,7 +2546,7 @@
         <v>0.5</v>
       </c>
       <c r="L24" t="str">
-        <f>A24&amp;"&amp;"&amp;'No. vertex and egg'!B21&amp;"&amp;"&amp;'No. vertex and egg'!C21&amp;"&amp;"&amp;IF(C24&lt;=I24,"\bf{"&amp;C24&amp;"}",C24)&amp;"&amp;"&amp;ROUND(D24,1)&amp;"&amp;"&amp;ROUND(E24,1)&amp;"&amp;"&amp;G24&amp;"&amp;"&amp;IF(I24&lt;=C24,"\bf{"&amp;I24&amp;"}",I24)&amp;"&amp;"&amp;ROUND(J24,1)&amp;"&amp;"&amp;IF(C53&lt;=I53,"\bf{"&amp;C53&amp;"}",C53)&amp;"&amp;"&amp;ROUND(D53,1)&amp;"&amp;"&amp;ROUND(E53,1)&amp;"&amp;"&amp;G53&amp;"&amp;"&amp;IF(I53&lt;=C53,"\bf{"&amp;I53&amp;"}",I53)&amp;"&amp;"&amp;ROUND(J53,1)&amp;"&amp;"&amp;IF(C82&lt;=I82,"\bf{"&amp;C82&amp;"}",C82)&amp;"&amp;"&amp;ROUND(D82,1)&amp;"&amp;"&amp;ROUND(E82,1)&amp;"&amp;"&amp;G82&amp;"&amp;"&amp;IF(I82&lt;=C82,"\bf{"&amp;I82&amp;"}",I82)&amp;"&amp;"&amp;ROUND(J82,1)&amp;"\\"</f>
+        <f>A24&amp;"&amp;"&amp;'No. vertex and egg'!B22&amp;"&amp;"&amp;'No. vertex and egg'!C22&amp;"&amp;"&amp;IF(C24&lt;=I24,"\bf{"&amp;C24&amp;"}",C24)&amp;"&amp;"&amp;ROUND(D24,1)&amp;"&amp;"&amp;ROUND(E24,1)&amp;"&amp;"&amp;G24&amp;"&amp;"&amp;IF(I24&lt;=C24,"\bf{"&amp;I24&amp;"}",I24)&amp;"&amp;"&amp;ROUND(J24,1)&amp;"&amp;"&amp;IF(C53&lt;=I53,"\bf{"&amp;C53&amp;"}",C53)&amp;"&amp;"&amp;ROUND(D53,1)&amp;"&amp;"&amp;ROUND(E53,1)&amp;"&amp;"&amp;G53&amp;"&amp;"&amp;IF(I53&lt;=C53,"\bf{"&amp;I53&amp;"}",I53)&amp;"&amp;"&amp;ROUND(J53,1)&amp;"&amp;"&amp;IF(C82&lt;=I82,"\bf{"&amp;C82&amp;"}",C82)&amp;"&amp;"&amp;ROUND(D82,1)&amp;"&amp;"&amp;ROUND(E82,1)&amp;"&amp;"&amp;G82&amp;"&amp;"&amp;IF(I82&lt;=C82,"\bf{"&amp;I82&amp;"}",I82)&amp;"&amp;"&amp;ROUND(J82,1)&amp;"\\"</f>
         <v>Belgrade&amp;19586&amp;7561185&amp;\bf{86.5}&amp;1.5&amp;1805.9&amp;PG&amp;103.4&amp;0.5&amp;\bf{171.1}&amp;2.4&amp;1803.8&amp;PG&amp;197.3&amp;0.9&amp;\bf{341.9}&amp;2.2&amp;1802.3&amp;SG&amp;374.5&amp;1.4\\</v>
       </c>
     </row>
@@ -1389,7 +2582,7 @@
         <v>0.5</v>
       </c>
       <c r="L25" t="str">
-        <f>A25&amp;"&amp;"&amp;'No. vertex and egg'!B22&amp;"&amp;"&amp;'No. vertex and egg'!C22&amp;"&amp;"&amp;IF(C25&lt;=I25,"\bf{"&amp;C25&amp;"}",C25)&amp;"&amp;"&amp;ROUND(D25,1)&amp;"&amp;"&amp;ROUND(E25,1)&amp;"&amp;"&amp;G25&amp;"&amp;"&amp;IF(I25&lt;=C25,"\bf{"&amp;I25&amp;"}",I25)&amp;"&amp;"&amp;ROUND(J25,1)&amp;"&amp;"&amp;IF(C54&lt;=I54,"\bf{"&amp;C54&amp;"}",C54)&amp;"&amp;"&amp;ROUND(D54,1)&amp;"&amp;"&amp;ROUND(E54,1)&amp;"&amp;"&amp;G54&amp;"&amp;"&amp;IF(I54&lt;=C54,"\bf{"&amp;I54&amp;"}",I54)&amp;"&amp;"&amp;ROUND(J54,1)&amp;"&amp;"&amp;IF(C83&lt;=I83,"\bf{"&amp;C83&amp;"}",C83)&amp;"&amp;"&amp;ROUND(D83,1)&amp;"&amp;"&amp;ROUND(E83,1)&amp;"&amp;"&amp;G83&amp;"&amp;"&amp;IF(I83&lt;=C83,"\bf{"&amp;I83&amp;"}",I83)&amp;"&amp;"&amp;ROUND(J83,1)&amp;"\\"</f>
+        <f>A25&amp;"&amp;"&amp;'No. vertex and egg'!B23&amp;"&amp;"&amp;'No. vertex and egg'!C23&amp;"&amp;"&amp;IF(C25&lt;=I25,"\bf{"&amp;C25&amp;"}",C25)&amp;"&amp;"&amp;ROUND(D25,1)&amp;"&amp;"&amp;ROUND(E25,1)&amp;"&amp;"&amp;G25&amp;"&amp;"&amp;IF(I25&lt;=C25,"\bf{"&amp;I25&amp;"}",I25)&amp;"&amp;"&amp;ROUND(J25,1)&amp;"&amp;"&amp;IF(C54&lt;=I54,"\bf{"&amp;C54&amp;"}",C54)&amp;"&amp;"&amp;ROUND(D54,1)&amp;"&amp;"&amp;ROUND(E54,1)&amp;"&amp;"&amp;G54&amp;"&amp;"&amp;IF(I54&lt;=C54,"\bf{"&amp;I54&amp;"}",I54)&amp;"&amp;"&amp;ROUND(J54,1)&amp;"&amp;"&amp;IF(C83&lt;=I83,"\bf{"&amp;C83&amp;"}",C83)&amp;"&amp;"&amp;ROUND(D83,1)&amp;"&amp;"&amp;ROUND(E83,1)&amp;"&amp;"&amp;G83&amp;"&amp;"&amp;IF(I83&lt;=C83,"\bf{"&amp;I83&amp;"}",I83)&amp;"&amp;"&amp;ROUND(J83,1)&amp;"\\"</f>
         <v>Berlin&amp;29461&amp;9944851&amp;\bf{102.1}&amp;1.9&amp;1817.9&amp;PG&amp;125.9&amp;0.5&amp;\bf{204.9}&amp;1.9&amp;1878.7&amp;PG&amp;240.1&amp;1.2&amp;\bf{396.4}&amp;3.1&amp;1804.8&amp;PG&amp;446.2&amp;1.8\\</v>
       </c>
     </row>
@@ -1425,7 +2618,7 @@
         <v>1.3</v>
       </c>
       <c r="L26" t="str">
-        <f>A26&amp;"&amp;"&amp;'No. vertex and egg'!B23&amp;"&amp;"&amp;'No. vertex and egg'!C23&amp;"&amp;"&amp;IF(C26&lt;=I26,"\bf{"&amp;C26&amp;"}",C26)&amp;"&amp;"&amp;ROUND(D26,1)&amp;"&amp;"&amp;ROUND(E26,1)&amp;"&amp;"&amp;G26&amp;"&amp;"&amp;IF(I26&lt;=C26,"\bf{"&amp;I26&amp;"}",I26)&amp;"&amp;"&amp;ROUND(J26,1)&amp;"&amp;"&amp;IF(C55&lt;=I55,"\bf{"&amp;C55&amp;"}",C55)&amp;"&amp;"&amp;ROUND(D55,1)&amp;"&amp;"&amp;ROUND(E55,1)&amp;"&amp;"&amp;G55&amp;"&amp;"&amp;IF(I55&lt;=C55,"\bf{"&amp;I55&amp;"}",I55)&amp;"&amp;"&amp;ROUND(J55,1)&amp;"&amp;"&amp;IF(C84&lt;=I84,"\bf{"&amp;C84&amp;"}",C84)&amp;"&amp;"&amp;ROUND(D84,1)&amp;"&amp;"&amp;ROUND(E84,1)&amp;"&amp;"&amp;G84&amp;"&amp;"&amp;IF(I84&lt;=C84,"\bf{"&amp;I84&amp;"}",I84)&amp;"&amp;"&amp;ROUND(J84,1)&amp;"\\"</f>
+        <f>A26&amp;"&amp;"&amp;'No. vertex and egg'!B24&amp;"&amp;"&amp;'No. vertex and egg'!C24&amp;"&amp;"&amp;IF(C26&lt;=I26,"\bf{"&amp;C26&amp;"}",C26)&amp;"&amp;"&amp;ROUND(D26,1)&amp;"&amp;"&amp;ROUND(E26,1)&amp;"&amp;"&amp;G26&amp;"&amp;"&amp;IF(I26&lt;=C26,"\bf{"&amp;I26&amp;"}",I26)&amp;"&amp;"&amp;ROUND(J26,1)&amp;"&amp;"&amp;IF(C55&lt;=I55,"\bf{"&amp;C55&amp;"}",C55)&amp;"&amp;"&amp;ROUND(D55,1)&amp;"&amp;"&amp;ROUND(E55,1)&amp;"&amp;"&amp;G55&amp;"&amp;"&amp;IF(I55&lt;=C55,"\bf{"&amp;I55&amp;"}",I55)&amp;"&amp;"&amp;ROUND(J55,1)&amp;"&amp;"&amp;IF(C84&lt;=I84,"\bf{"&amp;C84&amp;"}",C84)&amp;"&amp;"&amp;ROUND(D84,1)&amp;"&amp;"&amp;ROUND(E84,1)&amp;"&amp;"&amp;G84&amp;"&amp;"&amp;IF(I84&lt;=C84,"\bf{"&amp;I84&amp;"}",I84)&amp;"&amp;"&amp;ROUND(J84,1)&amp;"\\"</f>
         <v>Boston&amp;44797&amp;28164740&amp;\bf{94.3}&amp;1.9&amp;2391.9&amp;PG&amp;102.7&amp;1.3&amp;\bf{175.4}&amp;2&amp;2007&amp;PG&amp;191.6&amp;0.9&amp;\bf{341}&amp;0&amp;3819.2&amp;PG&amp;368.7&amp;1.5\\</v>
       </c>
     </row>
@@ -1461,7 +2654,7 @@
         <v>1.2</v>
       </c>
       <c r="L27" t="str">
-        <f>A27&amp;"&amp;"&amp;'No. vertex and egg'!B24&amp;"&amp;"&amp;'No. vertex and egg'!C24&amp;"&amp;"&amp;IF(C27&lt;=I27,"\bf{"&amp;C27&amp;"}",C27)&amp;"&amp;"&amp;ROUND(D27,1)&amp;"&amp;"&amp;ROUND(E27,1)&amp;"&amp;"&amp;G27&amp;"&amp;"&amp;IF(I27&lt;=C27,"\bf{"&amp;I27&amp;"}",I27)&amp;"&amp;"&amp;ROUND(J27,1)&amp;"&amp;"&amp;IF(C56&lt;=I56,"\bf{"&amp;C56&amp;"}",C56)&amp;"&amp;"&amp;ROUND(D56,1)&amp;"&amp;"&amp;ROUND(E56,1)&amp;"&amp;"&amp;G56&amp;"&amp;"&amp;IF(I56&lt;=C56,"\bf{"&amp;I56&amp;"}",I56)&amp;"&amp;"&amp;ROUND(J56,1)&amp;"&amp;"&amp;IF(C85&lt;=I85,"\bf{"&amp;C85&amp;"}",C85)&amp;"&amp;"&amp;ROUND(D85,1)&amp;"&amp;"&amp;ROUND(E85,1)&amp;"&amp;"&amp;G85&amp;"&amp;"&amp;IF(I85&lt;=C85,"\bf{"&amp;I85&amp;"}",I85)&amp;"&amp;"&amp;ROUND(J85,1)&amp;"\\"</f>
+        <f>A27&amp;"&amp;"&amp;'No. vertex and egg'!B25&amp;"&amp;"&amp;'No. vertex and egg'!C25&amp;"&amp;"&amp;IF(C27&lt;=I27,"\bf{"&amp;C27&amp;"}",C27)&amp;"&amp;"&amp;ROUND(D27,1)&amp;"&amp;"&amp;ROUND(E27,1)&amp;"&amp;"&amp;G27&amp;"&amp;"&amp;IF(I27&lt;=C27,"\bf{"&amp;I27&amp;"}",I27)&amp;"&amp;"&amp;ROUND(J27,1)&amp;"&amp;"&amp;IF(C56&lt;=I56,"\bf{"&amp;C56&amp;"}",C56)&amp;"&amp;"&amp;ROUND(D56,1)&amp;"&amp;"&amp;ROUND(E56,1)&amp;"&amp;"&amp;G56&amp;"&amp;"&amp;IF(I56&lt;=C56,"\bf{"&amp;I56&amp;"}",I56)&amp;"&amp;"&amp;ROUND(J56,1)&amp;"&amp;"&amp;IF(C85&lt;=I85,"\bf{"&amp;C85&amp;"}",C85)&amp;"&amp;"&amp;ROUND(D85,1)&amp;"&amp;"&amp;ROUND(E85,1)&amp;"&amp;"&amp;G85&amp;"&amp;"&amp;IF(I85&lt;=C85,"\bf{"&amp;I85&amp;"}",I85)&amp;"&amp;"&amp;ROUND(J85,1)&amp;"\\"</f>
         <v>Dublin&amp;37982&amp;21630466&amp;\bf{101.5}&amp;1.1&amp;1819.8&amp;PG&amp;113.8&amp;1.2&amp;\bf{193.2}&amp;4.8&amp;1815.9&amp;PG&amp;211.3&amp;2.7&amp;\bf{363}&amp;0&amp;3002.4&amp;PG&amp;390.2&amp;2\\</v>
       </c>
     </row>
@@ -1497,7 +2690,7 @@
         <v>0.9</v>
       </c>
       <c r="L28" t="str">
-        <f>A28&amp;"&amp;"&amp;'No. vertex and egg'!B25&amp;"&amp;"&amp;'No. vertex and egg'!C25&amp;"&amp;"&amp;IF(C28&lt;=I28,"\bf{"&amp;C28&amp;"}",C28)&amp;"&amp;"&amp;ROUND(D28,1)&amp;"&amp;"&amp;ROUND(E28,1)&amp;"&amp;"&amp;G28&amp;"&amp;"&amp;IF(I28&lt;=C28,"\bf{"&amp;I28&amp;"}",I28)&amp;"&amp;"&amp;ROUND(J28,1)&amp;"&amp;"&amp;IF(C57&lt;=I57,"\bf{"&amp;C57&amp;"}",C57)&amp;"&amp;"&amp;ROUND(D57,1)&amp;"&amp;"&amp;ROUND(E57,1)&amp;"&amp;"&amp;G57&amp;"&amp;"&amp;IF(I57&lt;=C57,"\bf{"&amp;I57&amp;"}",I57)&amp;"&amp;"&amp;ROUND(J57,1)&amp;"&amp;"&amp;IF(C86&lt;=I86,"\bf{"&amp;C86&amp;"}",C86)&amp;"&amp;"&amp;ROUND(D86,1)&amp;"&amp;"&amp;ROUND(E86,1)&amp;"&amp;"&amp;G86&amp;"&amp;"&amp;IF(I86&lt;=C86,"\bf{"&amp;I86&amp;"}",I86)&amp;"&amp;"&amp;ROUND(J86,1)&amp;"\\"</f>
+        <f>A28&amp;"&amp;"&amp;'No. vertex and egg'!B26&amp;"&amp;"&amp;'No. vertex and egg'!C26&amp;"&amp;"&amp;IF(C28&lt;=I28,"\bf{"&amp;C28&amp;"}",C28)&amp;"&amp;"&amp;ROUND(D28,1)&amp;"&amp;"&amp;ROUND(E28,1)&amp;"&amp;"&amp;G28&amp;"&amp;"&amp;IF(I28&lt;=C28,"\bf{"&amp;I28&amp;"}",I28)&amp;"&amp;"&amp;ROUND(J28,1)&amp;"&amp;"&amp;IF(C57&lt;=I57,"\bf{"&amp;C57&amp;"}",C57)&amp;"&amp;"&amp;ROUND(D57,1)&amp;"&amp;"&amp;ROUND(E57,1)&amp;"&amp;"&amp;G57&amp;"&amp;"&amp;IF(I57&lt;=C57,"\bf{"&amp;I57&amp;"}",I57)&amp;"&amp;"&amp;ROUND(J57,1)&amp;"&amp;"&amp;IF(C86&lt;=I86,"\bf{"&amp;C86&amp;"}",C86)&amp;"&amp;"&amp;ROUND(D86,1)&amp;"&amp;"&amp;ROUND(E86,1)&amp;"&amp;"&amp;G86&amp;"&amp;"&amp;IF(I86&lt;=C86,"\bf{"&amp;I86&amp;"}",I86)&amp;"&amp;"&amp;ROUND(J86,1)&amp;"\\"</f>
         <v>Minsk&amp;10487&amp;1375618&amp;\bf{102.1}&amp;1.1&amp;1801.5&amp;PG&amp;126&amp;0.9&amp;\bf{200}&amp;1.9&amp;1800.5&amp;PG&amp;240.4&amp;1.4&amp;\bf{387.7}&amp;3.5&amp;1801&amp;PG&amp;457.6&amp;2.4\\</v>
       </c>
     </row>
@@ -1556,7 +2749,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -1587,8 +2780,26 @@
       <c r="J33">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="P33" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>47</v>
+      </c>
+      <c r="R33" t="s">
+        <v>49</v>
+      </c>
+      <c r="S33" t="s">
+        <v>50</v>
+      </c>
+      <c r="T33" t="s">
+        <v>51</v>
+      </c>
+      <c r="U33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -1619,8 +2830,29 @@
       <c r="J34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O34" t="s">
+        <v>18</v>
+      </c>
+      <c r="P34">
+        <v>38</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>44.6</v>
+      </c>
+      <c r="R34">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="S34">
+        <v>89</v>
+      </c>
+      <c r="T34">
+        <v>140.1</v>
+      </c>
+      <c r="U34">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -1651,8 +2883,29 @@
       <c r="J35">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O35" t="s">
+        <v>19</v>
+      </c>
+      <c r="P35">
+        <v>39</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>50.2</v>
+      </c>
+      <c r="R35">
+        <v>76.3</v>
+      </c>
+      <c r="S35" s="7">
+        <v>97.6</v>
+      </c>
+      <c r="T35">
+        <v>148.30000000000001</v>
+      </c>
+      <c r="U35">
+        <v>179.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>21</v>
       </c>
@@ -1683,8 +2936,29 @@
       <c r="J36">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O36" t="s">
+        <v>20</v>
+      </c>
+      <c r="P36">
+        <v>21</v>
+      </c>
+      <c r="Q36" s="3">
+        <v>28.2</v>
+      </c>
+      <c r="R36">
+        <v>40.1</v>
+      </c>
+      <c r="S36" s="7">
+        <v>49.4</v>
+      </c>
+      <c r="T36">
+        <v>78</v>
+      </c>
+      <c r="U36">
+        <v>94.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -1715,8 +2989,29 @@
       <c r="J37">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O37" t="s">
+        <v>21</v>
+      </c>
+      <c r="P37">
+        <v>37</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>47.4</v>
+      </c>
+      <c r="R37">
+        <v>73.8</v>
+      </c>
+      <c r="S37" s="7">
+        <v>94</v>
+      </c>
+      <c r="T37">
+        <v>146.6</v>
+      </c>
+      <c r="U37">
+        <v>176.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -1747,8 +3042,29 @@
       <c r="J38">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O38" t="s">
+        <v>22</v>
+      </c>
+      <c r="P38">
+        <v>39</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>50.6</v>
+      </c>
+      <c r="R38">
+        <v>78.3</v>
+      </c>
+      <c r="S38" s="7">
+        <v>95.6</v>
+      </c>
+      <c r="T38">
+        <v>157.5</v>
+      </c>
+      <c r="U38">
+        <v>183.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -1779,8 +3095,29 @@
       <c r="J39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O39" t="s">
+        <v>23</v>
+      </c>
+      <c r="P39">
+        <v>38</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>44.8</v>
+      </c>
+      <c r="R39">
+        <v>73</v>
+      </c>
+      <c r="S39" s="8">
+        <v>85.1</v>
+      </c>
+      <c r="T39">
+        <v>149.19999999999999</v>
+      </c>
+      <c r="U39">
+        <v>172.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>25</v>
       </c>
@@ -1811,8 +3148,29 @@
       <c r="J40">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O40" t="s">
+        <v>24</v>
+      </c>
+      <c r="P40">
+        <v>38</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>50.6</v>
+      </c>
+      <c r="R40">
+        <v>77</v>
+      </c>
+      <c r="S40" s="8">
+        <v>95.7</v>
+      </c>
+      <c r="T40">
+        <v>158.1</v>
+      </c>
+      <c r="U40">
+        <v>182.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -1843,8 +3201,29 @@
       <c r="J41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O41" t="s">
+        <v>25</v>
+      </c>
+      <c r="P41">
+        <v>50.1</v>
+      </c>
+      <c r="Q41" s="3">
+        <v>59.2</v>
+      </c>
+      <c r="R41">
+        <v>94</v>
+      </c>
+      <c r="S41" s="8">
+        <v>110.6</v>
+      </c>
+      <c r="T41">
+        <v>175.2</v>
+      </c>
+      <c r="U41">
+        <v>199.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>27</v>
       </c>
@@ -1875,8 +3254,29 @@
       <c r="J42">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O42" t="s">
+        <v>26</v>
+      </c>
+      <c r="P42">
+        <v>40</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>52.4</v>
+      </c>
+      <c r="R42">
+        <v>79.5</v>
+      </c>
+      <c r="S42" s="7">
+        <v>99.6</v>
+      </c>
+      <c r="T42">
+        <v>152.80000000000001</v>
+      </c>
+      <c r="U42">
+        <v>187.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>28</v>
       </c>
@@ -1907,8 +3307,29 @@
       <c r="J43">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O43" t="s">
+        <v>27</v>
+      </c>
+      <c r="P43">
+        <v>38</v>
+      </c>
+      <c r="Q43" s="3">
+        <v>51.5</v>
+      </c>
+      <c r="R43">
+        <v>75</v>
+      </c>
+      <c r="S43" s="9">
+        <v>94.1</v>
+      </c>
+      <c r="T43">
+        <v>149.30000000000001</v>
+      </c>
+      <c r="U43">
+        <v>177.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>29</v>
       </c>
@@ -1939,8 +3360,29 @@
       <c r="J44">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O44" t="s">
+        <v>28</v>
+      </c>
+      <c r="P44">
+        <v>28</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>38.4</v>
+      </c>
+      <c r="R44">
+        <v>57</v>
+      </c>
+      <c r="S44" s="9">
+        <v>72</v>
+      </c>
+      <c r="T44">
+        <v>112.8</v>
+      </c>
+      <c r="U44">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>30</v>
       </c>
@@ -1971,8 +3413,29 @@
       <c r="J45">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O45" t="s">
+        <v>29</v>
+      </c>
+      <c r="P45">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="Q45" s="3">
+        <v>45.9</v>
+      </c>
+      <c r="R45">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="S45" s="9">
+        <v>91.5</v>
+      </c>
+      <c r="T45">
+        <v>155.19999999999999</v>
+      </c>
+      <c r="U45">
+        <v>178.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -2003,8 +3466,29 @@
       <c r="J46">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O46" t="s">
+        <v>30</v>
+      </c>
+      <c r="P46">
+        <v>44</v>
+      </c>
+      <c r="Q46" s="3">
+        <v>52.6</v>
+      </c>
+      <c r="R46">
+        <v>83.6</v>
+      </c>
+      <c r="S46" s="9">
+        <v>95.4</v>
+      </c>
+      <c r="T46">
+        <v>152.4</v>
+      </c>
+      <c r="U46">
+        <v>171.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>32</v>
       </c>
@@ -2035,8 +3519,29 @@
       <c r="J47">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O47" t="s">
+        <v>31</v>
+      </c>
+      <c r="P47">
+        <v>44</v>
+      </c>
+      <c r="Q47" s="3">
+        <v>56.6</v>
+      </c>
+      <c r="R47">
+        <v>84.7</v>
+      </c>
+      <c r="S47" s="9">
+        <v>103.3</v>
+      </c>
+      <c r="T47">
+        <v>164.2</v>
+      </c>
+      <c r="U47">
+        <v>195.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>33</v>
       </c>
@@ -2067,8 +3572,29 @@
       <c r="J48">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O48" t="s">
+        <v>32</v>
+      </c>
+      <c r="P48">
+        <v>24</v>
+      </c>
+      <c r="Q48" s="3">
+        <v>27.9</v>
+      </c>
+      <c r="R48">
+        <v>47</v>
+      </c>
+      <c r="S48" s="9">
+        <v>54.9</v>
+      </c>
+      <c r="T48">
+        <v>89</v>
+      </c>
+      <c r="U48">
+        <v>100.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>34</v>
       </c>
@@ -2099,8 +3625,29 @@
       <c r="J49">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O49" t="s">
+        <v>33</v>
+      </c>
+      <c r="P49">
+        <v>31</v>
+      </c>
+      <c r="Q49" s="3">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="R49">
+        <v>61.3</v>
+      </c>
+      <c r="S49" s="9">
+        <v>75</v>
+      </c>
+      <c r="T49">
+        <v>115.6</v>
+      </c>
+      <c r="U49">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -2131,8 +3678,29 @@
       <c r="J50">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O50" t="s">
+        <v>34</v>
+      </c>
+      <c r="P50">
+        <v>42</v>
+      </c>
+      <c r="Q50" s="3">
+        <v>52.5</v>
+      </c>
+      <c r="R50">
+        <v>84.6</v>
+      </c>
+      <c r="S50" s="9">
+        <v>98.9</v>
+      </c>
+      <c r="T50">
+        <v>161.4</v>
+      </c>
+      <c r="U50">
+        <v>182.2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -2163,8 +3731,29 @@
       <c r="J51">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O51" t="s">
+        <v>35</v>
+      </c>
+      <c r="P51">
+        <v>25</v>
+      </c>
+      <c r="Q51" s="3">
+        <v>29.6</v>
+      </c>
+      <c r="R51">
+        <v>49.2</v>
+      </c>
+      <c r="S51" s="9">
+        <v>61.1</v>
+      </c>
+      <c r="T51">
+        <v>97.6</v>
+      </c>
+      <c r="U51">
+        <v>113.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -2195,8 +3784,29 @@
       <c r="J52">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O52" t="s">
+        <v>36</v>
+      </c>
+      <c r="P52">
+        <v>36</v>
+      </c>
+      <c r="Q52" s="3">
+        <v>46.3</v>
+      </c>
+      <c r="R52">
+        <v>73</v>
+      </c>
+      <c r="S52" s="9">
+        <v>89.1</v>
+      </c>
+      <c r="T52">
+        <v>141</v>
+      </c>
+      <c r="U52">
+        <v>163.6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -2227,8 +3837,29 @@
       <c r="J53">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O53" t="s">
+        <v>37</v>
+      </c>
+      <c r="P53">
+        <v>32</v>
+      </c>
+      <c r="Q53" s="3">
+        <v>39.1</v>
+      </c>
+      <c r="R53">
+        <v>68</v>
+      </c>
+      <c r="S53" s="9">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="T53">
+        <v>130.4</v>
+      </c>
+      <c r="U53">
+        <v>145.80000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>39</v>
       </c>
@@ -2260,7 +3891,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>40</v>
       </c>
@@ -2291,8 +3922,26 @@
       <c r="J55">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="P55" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>47</v>
+      </c>
+      <c r="R55" t="s">
+        <v>49</v>
+      </c>
+      <c r="S55" t="s">
+        <v>50</v>
+      </c>
+      <c r="T55" t="s">
+        <v>51</v>
+      </c>
+      <c r="U55" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>41</v>
       </c>
@@ -2323,8 +3972,29 @@
       <c r="J56">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O56" t="s">
+        <v>38</v>
+      </c>
+      <c r="P56">
+        <v>86.5</v>
+      </c>
+      <c r="Q56">
+        <v>103.4</v>
+      </c>
+      <c r="R56">
+        <v>171.1</v>
+      </c>
+      <c r="S56">
+        <v>197.3</v>
+      </c>
+      <c r="T56">
+        <v>341.9</v>
+      </c>
+      <c r="U56">
+        <v>374.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>42</v>
       </c>
@@ -2355,25 +4025,109 @@
       <c r="J57" s="4">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O57" t="s">
+        <v>39</v>
+      </c>
+      <c r="P57">
+        <v>102.1</v>
+      </c>
+      <c r="Q57">
+        <v>125.9</v>
+      </c>
+      <c r="R57">
+        <v>204.9</v>
+      </c>
+      <c r="S57">
+        <v>240.1</v>
+      </c>
+      <c r="T57">
+        <v>396.4</v>
+      </c>
+      <c r="U57">
+        <v>446.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
-    </row>
-    <row r="59" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="O58" t="s">
+        <v>40</v>
+      </c>
+      <c r="P58">
+        <v>94.3</v>
+      </c>
+      <c r="Q58">
+        <v>102.7</v>
+      </c>
+      <c r="R58">
+        <v>175.4</v>
+      </c>
+      <c r="S58">
+        <v>191.6</v>
+      </c>
+      <c r="T58">
+        <v>341</v>
+      </c>
+      <c r="U58">
+        <v>368.7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="O59" t="s">
+        <v>41</v>
+      </c>
+      <c r="P59">
+        <v>101.5</v>
+      </c>
+      <c r="Q59">
+        <v>113.8</v>
+      </c>
+      <c r="R59">
+        <v>193.2</v>
+      </c>
+      <c r="S59">
+        <v>211.3</v>
+      </c>
+      <c r="T59">
+        <v>363</v>
+      </c>
+      <c r="U59" s="4">
+        <v>390.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G60" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O60" t="s">
+        <v>42</v>
+      </c>
+      <c r="P60">
+        <v>102.1</v>
+      </c>
+      <c r="Q60" s="4">
+        <v>126</v>
+      </c>
+      <c r="R60">
+        <v>200</v>
+      </c>
+      <c r="S60" s="4">
+        <v>240.4</v>
+      </c>
+      <c r="T60">
+        <v>387.7</v>
+      </c>
+      <c r="U60" s="4">
+        <v>457.6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>1</v>
       </c>
@@ -2405,7 +4159,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>18</v>
       </c>
@@ -2437,7 +4191,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>19</v>
       </c>
@@ -2469,7 +4223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>20</v>
       </c>
@@ -3207,292 +4961,300 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1">
-        <v>910</v>
-      </c>
-      <c r="C1">
-        <v>18560</v>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2">
-        <v>1700</v>
+        <v>910</v>
       </c>
       <c r="C2">
-        <v>62617</v>
+        <v>18560</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3">
-        <v>976</v>
+        <v>1700</v>
       </c>
       <c r="C3">
-        <v>35012</v>
+        <v>62617</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>1569</v>
+        <v>976</v>
       </c>
       <c r="C4">
-        <v>47522</v>
+        <v>35012</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5">
-        <v>1127</v>
+        <v>1569</v>
       </c>
       <c r="C5">
-        <v>23155</v>
+        <v>47522</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6">
-        <v>1175</v>
+        <v>1127</v>
       </c>
       <c r="C6">
-        <v>26689</v>
+        <v>23155</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7">
-        <v>1250</v>
+        <v>1175</v>
       </c>
       <c r="C7">
-        <v>31997</v>
+        <v>26689</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8">
-        <v>1137</v>
+        <v>1250</v>
       </c>
       <c r="C8">
-        <v>24323</v>
+        <v>31997</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9">
-        <v>1647</v>
+        <v>1137</v>
       </c>
       <c r="C9">
-        <v>56511</v>
+        <v>24323</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10">
-        <v>1531</v>
+        <v>1647</v>
       </c>
       <c r="C10">
-        <v>48219</v>
+        <v>56511</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11">
-        <v>1273</v>
+        <v>1531</v>
       </c>
       <c r="C11">
-        <v>42564</v>
+        <v>48219</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12">
-        <v>1991</v>
+        <v>1273</v>
       </c>
       <c r="C12">
-        <v>77286</v>
+        <v>42564</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13">
-        <v>1109</v>
+        <v>1991</v>
       </c>
       <c r="C13">
-        <v>26614</v>
+        <v>77286</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14">
-        <v>1739</v>
+        <v>1109</v>
       </c>
       <c r="C14">
-        <v>51595</v>
+        <v>26614</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15">
-        <v>479</v>
+        <v>1739</v>
       </c>
       <c r="C15">
-        <v>8396</v>
+        <v>51595</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16">
-        <v>1122</v>
+        <v>479</v>
       </c>
       <c r="C16">
-        <v>35070</v>
+        <v>8396</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17">
-        <v>1582</v>
+        <v>1122</v>
       </c>
       <c r="C17">
-        <v>50534</v>
+        <v>35070</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18">
-        <v>796</v>
+        <v>1582</v>
       </c>
       <c r="C18">
-        <v>19942</v>
+        <v>50534</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19">
-        <v>1346</v>
+        <v>796</v>
       </c>
       <c r="C19">
-        <v>42013</v>
+        <v>19942</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20">
-        <v>1044</v>
+        <v>1346</v>
       </c>
       <c r="C20">
-        <v>23774</v>
+        <v>42013</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21">
-        <v>19586</v>
+        <v>1044</v>
       </c>
       <c r="C21">
-        <v>7561185</v>
+        <v>23774</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22">
-        <v>29461</v>
+        <v>19586</v>
       </c>
       <c r="C22">
-        <v>9944851</v>
+        <v>7561185</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23">
-        <v>44797</v>
+        <v>29461</v>
       </c>
       <c r="C23">
-        <v>28164740</v>
+        <v>9944851</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24">
-        <v>37982</v>
+        <v>44797</v>
       </c>
       <c r="C24">
-        <v>21630466</v>
+        <v>28164740</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25">
+        <v>37982</v>
+      </c>
+      <c r="C25">
+        <v>21630466</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>42</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>10487</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>1375618</v>
       </c>
     </row>
@@ -3501,5 +5263,6 @@
     <sortCondition ref="C20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>